<commit_message>
Modified IOPS Per User: Now user entered
IOPS per user is user-entered with a limit of 1 - 200
Recommendations are provided
</commit_message>
<xml_diff>
--- a/fslogix-storage-calculator.xlsx
+++ b/fslogix-storage-calculator.xlsx
@@ -8,8 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netapp-my.sharepoint.com/personal/mchad_netapp_com/Documents/Documents/DataFabric/calculators/fslogix-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{80057BE8-5265-429A-8C17-C870DB06A720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3C11F1FD-C863-4404-8DB4-01D61EAB8F75}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="N7T0sGOloLfdFA83WVOXPOPZejpNmZwOJdFFNuEXibIHfqr4mztCFetwCvHQSbUmHxB7tAnm8eiXYgqOYWHzDA==" workbookSaltValue="2fErBk1//dUDK2o4yEmquw==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{80057BE8-5265-429A-8C17-C870DB06A720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{139D8C4D-F01E-4B3F-83D6-81314EE328FE}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="t+JkNq9tqmsPWKZG4243dmROwKF3bq/0/pMp0U7P3IbsgB19gsMVOhnXvXvDRyuLi2nqOQxBUhOjuGiZBOrHlQ==" workbookSaltValue="OSy8GVs1Yity0kiwcucv5A==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{CB3913B2-BB8F-4CB3-9459-2FD527F7F31B}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>IOPS Per User</t>
   </si>
   <si>
-    <t>Drop Down: IOPS Per User</t>
-  </si>
-  <si>
     <t>Fields</t>
   </si>
   <si>
@@ -548,6 +545,9 @@
   </si>
   <si>
     <t>Max Total Supported User Count (Based on Concurrent I/O Rate)</t>
+  </si>
+  <si>
+    <t>Modify: IOPS Per User</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00000000_);[Red]\(&quot;$&quot;#,##0.00000000\)"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,14 +601,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -732,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -893,7 +885,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -943,21 +934,6 @@
   </cellStyles>
   <dxfs count="98">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1116,6 +1092,349 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1443,334 +1762,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3616,7 +3607,6 @@
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
-      <sheetData sheetId="8" refreshError="1"/>
       <sheetData sheetId="9">
         <row r="2">
           <cell r="G2" t="str">
@@ -3911,84 +3901,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{856F6794-4173-4194-B8E4-7BB540367D16}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{856F6794-4173-4194-B8E4-7BB540367D16}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96" tableBorderDxfId="95">
   <autoFilter ref="A2:B9" xr:uid="{91E6A135-C0E7-4D0B-8EB4-141892DA45C5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2F564818-5A0F-4075-8D5E-BCEC57D8FC3C}" name="Fields" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{D42113E7-14D7-4A36-BB89-433CD657FB9D}" name="Input " dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{2F564818-5A0F-4075-8D5E-BCEC57D8FC3C}" name="Fields" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{D42113E7-14D7-4A36-BB89-433CD657FB9D}" name="Input " dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5554924-003B-4661-B33F-97EE2DB8E4A1}" name="Table8" displayName="Table8" ref="A22:B47" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5554924-003B-4661-B33F-97EE2DB8E4A1}" name="Table8" displayName="Table8" ref="A22:B47" totalsRowShown="0" dataDxfId="55">
   <autoFilter ref="A22:B47" xr:uid="{783E58C8-C7D9-4121-86C6-A6F7E49A97E3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{62872274-DD35-4869-BA93-32B33621B006}" name="Keys" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{BCBEE816-C2FF-4BB7-8812-71E8D95CE734}" name="Values" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{62872274-DD35-4869-BA93-32B33621B006}" name="Keys" dataDxfId="54"/>
+    <tableColumn id="2" xr3:uid="{BCBEE816-C2FF-4BB7-8812-71E8D95CE734}" name="Values" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E152E804-6E16-4FE5-822A-359F4049D3B1}" name="Table2" displayName="Table2" ref="A28:B32" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E152E804-6E16-4FE5-822A-359F4049D3B1}" name="Table2" displayName="Table2" ref="A28:B32" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" tableBorderDxfId="90">
   <autoFilter ref="A28:B32" xr:uid="{4897B486-AB3B-4450-B296-0E35971B3AE2}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3A7044B6-6E00-4BEF-9FE6-A7DEE00EE3F3}" name="Azure Files Price Break Down" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{6BB28A88-2884-4CC5-80B3-4CA3051CCAC3}" name="Calculated Output" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{3A7044B6-6E00-4BEF-9FE6-A7DEE00EE3F3}" name="Azure Files Price Break Down" dataDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{6BB28A88-2884-4CC5-80B3-4CA3051CCAC3}" name="Calculated Output" dataDxfId="88"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BA317605-A8C7-4DFA-9894-A955BD37C1CF}" name="Table4" displayName="Table4" ref="A11:B16" totalsRowShown="0" headerRowDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BA317605-A8C7-4DFA-9894-A955BD37C1CF}" name="Table4" displayName="Table4" ref="A11:B16" totalsRowShown="0" headerRowDxfId="87" tableBorderDxfId="86">
   <autoFilter ref="A11:B16" xr:uid="{FDD62D26-CF49-4DB8-BB86-E5640AFB3072}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{98F6AE4C-A8FE-46A2-B695-4F7EC29B79C1}" name="High Level Environmental Needs" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{923448D6-8587-46CF-AC83-4786C0E6E31A}" name="Calculated Output" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{98F6AE4C-A8FE-46A2-B695-4F7EC29B79C1}" name="High Level Environmental Needs" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{923448D6-8587-46CF-AC83-4786C0E6E31A}" name="Calculated Output" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E9B81EED-ACF0-4F74-94BF-2331D9B58AEF}" name="Table5" displayName="Table5" ref="A36:B38" totalsRowShown="0" dataDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E9B81EED-ACF0-4F74-94BF-2331D9B58AEF}" name="Table5" displayName="Table5" ref="A36:B38" totalsRowShown="0" dataDxfId="83" tableBorderDxfId="82">
   <autoFilter ref="A36:B38" xr:uid="{F64951B7-0541-475C-8E4E-15CB609631E0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EEA382B5-FB82-4F1D-9327-A87385C52897}" name="Azure Premium Files Price Break Down" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{E770553C-A0C0-45E6-BC23-3E0DD3249B14}" name="Calculated Output" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{EEA382B5-FB82-4F1D-9327-A87385C52897}" name="Azure Premium Files Price Break Down" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{E770553C-A0C0-45E6-BC23-3E0DD3249B14}" name="Calculated Output" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{72039F74-6304-436F-9B2C-E726744D9970}" name="Table9" displayName="Table9" ref="A18:B22" totalsRowShown="0" dataDxfId="42" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{72039F74-6304-436F-9B2C-E726744D9970}" name="Table9" displayName="Table9" ref="A18:B22" totalsRowShown="0" dataDxfId="79" tableBorderDxfId="78">
   <autoFilter ref="A18:B22" xr:uid="{1849FF8B-C5DF-48B3-BD49-7E1B6D720287}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3F78E685-9C28-44F6-9A2A-3F9135F54C28}" name="Azure NetApp Files Price Break Down" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{AA370671-CA18-4101-A4C3-7BC422CCC1F1}" name="Calculated Output" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{3F78E685-9C28-44F6-9A2A-3F9135F54C28}" name="Azure NetApp Files Price Break Down" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{AA370671-CA18-4101-A4C3-7BC422CCC1F1}" name="Calculated Output" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{2F4EE936-97FF-430B-BCE0-3BA4433FF3D4}" name="Table91119" displayName="Table91119" ref="D18:H26" totalsRowShown="0" dataDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{2F4EE936-97FF-430B-BCE0-3BA4433FF3D4}" name="Table91119" displayName="Table91119" ref="D18:H26" totalsRowShown="0" dataDxfId="75" tableBorderDxfId="74">
   <autoFilter ref="D18:H26" xr:uid="{F75E429C-8018-41C4-B4C3-C0AD783F2D38}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{25D43E32-76CE-4E57-9637-4A7FD2463E37}" name="Azure NetApp Files Additional Information" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{3C9CF5B6-EAB8-4222-9C96-5A10EE28F85F}" name=" Output" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{F8FAE1CB-5733-4CC5-9F68-AD29EB511AF6}" name="Etc(1)" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{25D43E32-76CE-4E57-9637-4A7FD2463E37}" name="Azure NetApp Files Additional Information" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{3C9CF5B6-EAB8-4222-9C96-5A10EE28F85F}" name=" Output" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{F8FAE1CB-5733-4CC5-9F68-AD29EB511AF6}" name="Etc(1)" dataDxfId="70">
       <calculatedColumnFormula>IF(E20&gt;definitions!B24,definitions!$A$23,"Yes")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2A8935D0-2756-4A0D-B01F-87C8DFAE1AD5}" name="Etc(2)" dataDxfId="32">
+    <tableColumn id="4" xr3:uid="{2A8935D0-2756-4A0D-B01F-87C8DFAE1AD5}" name="Etc(2)" dataDxfId="69">
       <calculatedColumnFormula>IF(B3&gt;E24,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7CD54AC1-822B-4FE1-B7D3-C9A779DEF8FC}" name="Etc(3)" dataDxfId="31">
+    <tableColumn id="5" xr3:uid="{7CD54AC1-822B-4FE1-B7D3-C9A779DEF8FC}" name="Etc(3)" dataDxfId="68">
       <calculatedColumnFormula>IF(B3&gt;E24,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3997,18 +3987,18 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{E617B910-6016-4284-B1B7-B2BDBB2DAC94}" name="Table622" displayName="Table622" ref="D28:H34" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{E617B910-6016-4284-B1B7-B2BDBB2DAC94}" name="Table622" displayName="Table622" ref="D28:H34" totalsRowShown="0" headerRowDxfId="67" tableBorderDxfId="66">
   <autoFilter ref="D28:H34" xr:uid="{6432D5DC-E020-4F4A-81F0-AFAE2FFBB2FE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{284AB7F5-C1F5-4923-8D18-8B326F2B7795}" name="Azure Standard Files Additional Information"/>
-    <tableColumn id="2" xr3:uid="{A95529E7-EF42-4D6F-BDD9-4D129864E797}" name="Output" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{9881ABB1-4E08-4030-AEC9-CCA810605C29}" name="Etc(1)" dataDxfId="27">
+    <tableColumn id="2" xr3:uid="{A95529E7-EF42-4D6F-BDD9-4D129864E797}" name="Output" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{9881ABB1-4E08-4030-AEC9-CCA810605C29}" name="Etc(1)" dataDxfId="64">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5BC3DEF6-CDB9-4DE9-B8FF-9749CBA220CD}" name="Etc(2)" dataDxfId="26">
+    <tableColumn id="4" xr3:uid="{5BC3DEF6-CDB9-4DE9-B8FF-9749CBA220CD}" name="Etc(2)" dataDxfId="63">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3F802064-6239-4D79-9EEF-E6B1422584F4}" name="Etc(3)" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{3F802064-6239-4D79-9EEF-E6B1422584F4}" name="Etc(3)" dataDxfId="62">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4017,15 +4007,15 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{017E12BE-FEED-449C-A993-3E3DA447FC83}" name="Table61423" displayName="Table61423" ref="D36:G42" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{017E12BE-FEED-449C-A993-3E3DA447FC83}" name="Table61423" displayName="Table61423" ref="D36:G42" totalsRowShown="0" headerRowDxfId="61" tableBorderDxfId="60">
   <autoFilter ref="D36:G42" xr:uid="{35197520-871D-45A1-92D2-3E64562C597C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7454E181-1F78-43D7-992D-393BF7E62908}" name="Azure Premium Files Additional Information"/>
-    <tableColumn id="2" xr3:uid="{D283543A-6DF3-46B8-B880-680345E5383E}" name="output" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{383E5A06-7313-4E3D-A474-C65E865DB16D}" name="Etc(1)" dataDxfId="21">
+    <tableColumn id="2" xr3:uid="{D283543A-6DF3-46B8-B880-680345E5383E}" name="output" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{383E5A06-7313-4E3D-A474-C65E865DB16D}" name="Etc(1)" dataDxfId="58">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{22B7B0DB-CD46-43E2-A4B8-192176C63B53}" name="Etc(2)" dataDxfId="20">
+    <tableColumn id="4" xr3:uid="{22B7B0DB-CD46-43E2-A4B8-192176C63B53}" name="Etc(2)" dataDxfId="57">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4040,7 +4030,7 @@
     <tableColumn id="2" xr3:uid="{9191646A-D382-43C8-AD5D-D9379A6352B8}" name="IO Size"/>
     <tableColumn id="3" xr3:uid="{B94E1025-3714-4DA4-824F-A38F565F77F4}" name="IOPS Per User"/>
     <tableColumn id="1" xr3:uid="{E67A9471-95D1-42FF-B18E-7D012DE67FD4}" name="VHD Sizes"/>
-    <tableColumn id="4" xr3:uid="{779397D8-86EA-41AE-9217-A6D49A13139B}" name="Concurrent Users" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{779397D8-86EA-41AE-9217-A6D49A13139B}" name="Concurrent Users" dataDxfId="56"/>
     <tableColumn id="5" xr3:uid="{5EBEBC80-5940-4420-B7CB-91D5FC7DF075}" name="Read Percenage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4349,13 +4339,13 @@
   </sheetPr>
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" customWidth="1"/>
     <col min="4" max="4" width="85.42578125" bestFit="1" customWidth="1"/>
@@ -4366,17 +4356,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="79"/>
+      <c r="A1" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="78"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4386,20 +4376,19 @@
       <c r="B3" s="32">
         <v>118</v>
       </c>
-      <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="B4" s="32">
         <v>15</v>
       </c>
-      <c r="D4" s="63"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="32">
         <v>35</v>
@@ -4407,7 +4396,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B6" s="47">
         <v>1</v>
@@ -4416,26 +4405,26 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="32">
         <v>40</v>
       </c>
-      <c r="D7" s="76"/>
+      <c r="D7" s="75"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="32">
         <v>32</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" s="62">
         <v>0.2</v>
@@ -4447,15 +4436,15 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="18">
         <f>B$3*B$6</f>
@@ -4464,7 +4453,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="18">
         <f>(B$4*B$8*B$3*B$6)/1024</f>
@@ -4473,7 +4462,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="18">
         <f>(B$4*B$8)</f>
@@ -4482,7 +4471,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="18">
         <f>B$4*B$3*B6</f>
@@ -4491,7 +4480,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="18">
         <f>B5*B3</f>
@@ -4499,50 +4488,50 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="80" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="80"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
+      <c r="A17" s="79" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="79"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="79"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" t="s">
         <v>58</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>59</v>
-      </c>
-      <c r="H18" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="51" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="54">
         <f>IF(E19="Yes",_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!C$38:C$40,'Azure NetApp Files Calcuations'!B$38:B$40,definitions!A$23),"N/A: User Count Excceds Capability Of Azure NetApp Files")</f>
         <v>619.5</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="48" t="str">
         <f>_xlfn.XLOOKUP("No",'Azure NetApp Files Calcuations'!B35:B36,'Azure NetApp Files Calcuations'!B35:B36,"Yes")</f>
@@ -4552,116 +4541,116 @@
         <f>IF('Azure NetApp Files Calcuations'!B35="Yes","Yes",definitions!$A$23)</f>
         <v>Yes</v>
       </c>
-      <c r="G19" s="67"/>
-      <c r="H19" s="66" t="str">
+      <c r="G19" s="66"/>
+      <c r="H19" s="65" t="str">
         <f>IF(B3&gt;E24,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</f>
         <v>Yes</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="49">
         <f>IF(E19="Yes",IF($E$21=definitions!A$23,B$19,B$19/B$3),"N/A: User Count Excceds Capability Of Azure NetApp Files")</f>
         <v>5.25</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E20" s="52">
         <f>IF('Azure NetApp Files Calcuations'!B35="Yes",_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!$C$31:$C$33,'Azure NetApp Files Calcuations'!$B$31:$B$33),"No")</f>
         <v>4130</v>
       </c>
       <c r="F20" s="53"/>
-      <c r="G20" s="68"/>
-      <c r="H20" s="68"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
     </row>
     <row r="21" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="50">
         <f>IF(E29="Yes",_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!C$46:C$48,'Azure NetApp Files Calcuations'!B$46:B$48),"N/A: User Count Exceeds Capability Of Azure Files")</f>
         <v>1.4982876712328768</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E21" s="52" t="str">
         <f>IF('Azure NetApp Files Calcuations'!B35="Yes",(_xlfn.XLOOKUP(MIN('Azure NetApp Files Calcuations'!$B$38:$B$40),'Azure NetApp Files Calcuations'!$B$38:$B$40,'Azure NetApp Files Calcuations'!$C$38:$C$40)),"No")</f>
         <v>Standard</v>
       </c>
       <c r="F21" s="53"/>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
     </row>
     <row r="22" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="50">
         <f>IF(E37="Yes",_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!C$50:C$52,'Azure NetApp Files Calcuations'!B$50:B$52),"N/A: User Count Exceeds Capability Of Azure Premium Files")</f>
         <v>0.6</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E22" s="52" t="str">
         <f>IF(E19="No","No",(_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!$C$27:$C$29,'Azure NetApp Files Calcuations'!$B$27:$B$29)))</f>
         <v>Capacity</v>
       </c>
       <c r="F22" s="53"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
     </row>
     <row r="23" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="35"/>
       <c r="B23" s="50"/>
       <c r="D23" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" s="52">
         <f>IF(E19="Yes",(_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!$C$42:$C$44,'Azure NetApp Files Calcuations'!$B$42:$B$44,definitions!A$23)),"No")</f>
         <v>35</v>
       </c>
       <c r="F23" s="53"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
     </row>
     <row r="24" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="49"/>
-      <c r="D24" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="E24" s="70">
+      <c r="D24" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="69">
         <f>FLOOR(('Azure NetApp Files Calcuations'!B4*1024/'FSLogix Calculator'!B14)*(1/'FSLogix Calculator'!B6),1)</f>
         <v>4689</v>
       </c>
-      <c r="F24" s="69"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
     </row>
     <row r="25" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35"/>
       <c r="B25" s="49"/>
-      <c r="D25" s="65" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25" s="70">
+      <c r="D25" s="64" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="69">
         <f>'Azure NetApp Files Calcuations'!B5</f>
         <v>2925</v>
       </c>
-      <c r="F25" s="69" t="str">
+      <c r="F25" s="68" t="str">
         <f>IF(E26&gt;definitions!B30,definitions!$A$23,"Yes")</f>
         <v>Required capacity exceeds documented 100TiB upper limit</v>
       </c>
-      <c r="G25" s="69" t="str">
+      <c r="G25" s="68" t="str">
         <f>IF(B9&gt;E28,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</f>
         <v>Yes</v>
       </c>
-      <c r="H25" s="69" t="str">
+      <c r="H25" s="68" t="str">
         <f>IF(B9&gt;E28,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</f>
         <v>Yes</v>
       </c>
@@ -4677,61 +4666,61 @@
         <f>IF(E22="Capacity Pool Minimum Size",_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!$C$15:$C$17,'Azure NetApp Files Calcuations'!$B$15:$B$17),"Temporarily Empty Field")</f>
         <v>Temporarily Empty Field</v>
       </c>
-      <c r="F26" s="64"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
     </row>
     <row r="27" spans="1:8" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="80" t="s">
-        <v>86</v>
-      </c>
-      <c r="B27" s="80"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="80"/>
-      <c r="H27" s="80"/>
+      <c r="A27" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F28" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="G28" s="58" t="s">
+      <c r="H28" s="58" t="s">
         <v>59</v>
-      </c>
-      <c r="H28" s="58" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="54">
         <f>IF(E29="Yes",B$32+B$31,"N/A: User Count Exceeds Capability Of Azure Files")</f>
         <v>413.47199999999998</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="35" t="str">
         <f>_xlfn.XLOOKUP("No",'Azure Files Calculations'!$C$2:$C$4,'Azure Files Calculations'!$C$2:$C$4,"Yes")</f>
         <v>Yes</v>
       </c>
-      <c r="F29" s="72" t="str">
+      <c r="F29" s="71" t="str">
         <f>'Azure Files Calculations'!$B$4</f>
         <v>Yes</v>
       </c>
@@ -4746,14 +4735,14 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="49">
         <f>IF(E29="Yes",B$29/B$3,"N/A: User Count Exceeds Capability Of Azure Files")</f>
         <v>3.504</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" s="18">
         <f>IF(E29="Yes",$B$5*$B$3,"No")</f>
@@ -4765,14 +4754,14 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="49">
         <f>IF(E29="Yes",((B4*B3*B6*definitions!B$32*B$7*definitions!B$34)/definitions!B33)*definitions!B$36,"N/A: User Count Exceeds Capability Of Azure Files")</f>
         <v>165.672</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E31" s="18">
         <f>IF(E29="Yes",E30/$B$3,"No")</f>
@@ -4784,14 +4773,14 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="49">
         <f>IF(E29="Yes",B$5*B$3*B6*definitions!B$35,"N/A: User Count Exceeds Capability Of Azure Files")</f>
         <v>247.79999999999998</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E32" s="18">
         <f>FLOOR(   (definitions!$B$38/$B$4)*(1/$B$6),1)</f>
@@ -4805,7 +4794,7 @@
       <c r="A33" s="35"/>
       <c r="B33" s="49"/>
       <c r="D33" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E33" s="18">
         <f>FLOOR((   (1024*definitions!$B$39)   /   ('FSLogix Calculator'!$B$4*'FSLogix Calculator'!$B$8)  ) * (1/$B$6   ),1)</f>
@@ -4816,82 +4805,82 @@
       <c r="H33" s="40"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D34" s="65" t="s">
-        <v>151</v>
+      <c r="D34" s="64" t="s">
+        <v>150</v>
       </c>
       <c r="E34" s="17">
         <f>definitions!B41/'FSLogix Calculator'!B5</f>
         <v>2925.7142857142858</v>
       </c>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
     </row>
     <row r="35" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="80" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="80"/>
-      <c r="C35" s="80"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="80"/>
-      <c r="G35" s="80"/>
+      <c r="A35" s="79" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
+      <c r="D35" s="79"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="79"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F36" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" t="s">
         <v>58</v>
-      </c>
-      <c r="G36" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="54">
         <f>IF(E37="Yes",IF(E40="I/O Need",definitions!B37*'FSLogix Calculator'!B3*'FSLogix Calculator'!B4,definitions!B37*'FSLogix Calculator'!B5*'FSLogix Calculator'!B3),"N/A: User Count Exceeds Capability Of Azure Premium Files")</f>
         <v>1032.5</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E37" s="35" t="str">
         <f>_xlfn.XLOOKUP("No",'Azure Files Calculations'!$C$5:$C$7,'Azure Files Calculations'!$C$2:$C$4,"Yes")</f>
         <v>Yes</v>
       </c>
-      <c r="F37" s="73" t="str">
+      <c r="F37" s="72" t="str">
         <f>'Azure Files Calculations'!$B$6</f>
         <v>Yes</v>
       </c>
-      <c r="G37" s="73" t="str">
+      <c r="G37" s="72" t="str">
         <f>'Azure Files Calculations'!$B$5</f>
         <v>Yes</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" s="23">
         <f>IF(E37="Yes",B$37/B$3,"N/A: User Count Exceeds Capability Of Azure Premium Files")</f>
         <v>8.75</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E38" s="18">
         <f>'Azure Files Calculations'!C14</f>
@@ -4902,7 +4891,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E39" s="17">
         <f>IF('Azure Files Calculations'!$C$6="Yes",E$38/$B$3,"No")</f>
@@ -4916,7 +4905,7 @@
       <c r="B40" s="17"/>
       <c r="C40" s="8"/>
       <c r="D40" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E40" s="22" t="str">
         <f>'Azure Files Calculations'!B14</f>
@@ -4930,7 +4919,7 @@
       <c r="B41" s="17"/>
       <c r="C41" s="8"/>
       <c r="D41" s="27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E41" s="18">
         <f>FLOOR(( definitions!$B$40/$B$4) * (1/$B$6),1)</f>
@@ -4941,8 +4930,8 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="8"/>
-      <c r="D42" s="65" t="s">
-        <v>153</v>
+      <c r="D42" s="64" t="s">
+        <v>152</v>
       </c>
       <c r="E42" s="18">
         <f>definitions!B42/'FSLogix Calculator'!B5</f>
@@ -5195,7 +5184,7 @@
       <c r="E112" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="FA1HdkEUmZ4cjbh1PswAaQpeKciB3/Rjl997vG8Cyt1OIGa+ZgKkB4XbyikN3n2OB4tG6B3j47xSo6jvrb9o2Q==" saltValue="zkkTPd3CZsu4/tUUvkGJng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vjT6CCKfIrO/jXzdur1RhpGnjRqhL+DaQXy52zAi/TSyztQjEWBS2QXCVfbW28nJMhsff53LBSETI75V5qR4rw==" saltValue="dqYSPUVkn4pwwVpSznIOyA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A27:H27"/>
@@ -5204,167 +5193,167 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A36:B39 A28:B34">
-    <cfRule type="cellIs" dxfId="97" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="93" operator="equal">
       <formula>"Temporarily Empty Field"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:H31">
-    <cfRule type="containsText" dxfId="96" priority="23" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="51" priority="23" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="24" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="50" priority="24" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",F29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E23">
-    <cfRule type="cellIs" dxfId="94" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
       <formula>"Capacity Pool Minimum Size"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="93" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="40" operator="equal">
       <formula>"Temporarily Empty Field"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="92" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="39" operator="equal">
       <formula>"Temporarily Empty Field"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="91" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="31" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="32" operator="equal">
       <formula>"""Yes"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="38" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="88" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
       <formula>"Required Capacity Exceeds documented 100TiB Upper Limit"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="34" operator="equal">
       <formula>"""Required Capacity Exceeds documented 100TiB Upper Limit"""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="35" operator="containsText" text="&quot;Required&quot;">
+    <cfRule type="containsText" dxfId="41" priority="35" operator="containsText" text="&quot;Required&quot;">
       <formula>NOT(ISERROR(SEARCH("""Required""",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="36" operator="containsText" text="&quot;Required&quot;">
+    <cfRule type="containsText" dxfId="40" priority="36" operator="containsText" text="&quot;Required&quot;">
       <formula>NOT(ISERROR(SEARCH("""Required""",F19)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="83" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="29" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="30" operator="equal">
       <formula>"No: 300MiB/s is Maximum Supported Load"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="81" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="80" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="27" operator="equal">
       <formula>"""No: 102,400GiB is Maximum Supported Capacity"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="79" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="25" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="26" operator="equal">
       <formula>"No: 102,400GiB is Maximum Supported Capacity"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37 E40">
-    <cfRule type="cellIs" dxfId="77" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="21" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="22" operator="equal">
       <formula>"No: 100,000 IOPS is Maximum Supported Load"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37:G38 F40:G40">
-    <cfRule type="containsText" dxfId="75" priority="18" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="30" priority="18" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",F37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="29" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37 E40">
-    <cfRule type="cellIs" dxfId="73" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="19" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31 E20:E23">
-    <cfRule type="cellIs" dxfId="72" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="71" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="70" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="69" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="containsText" dxfId="68" priority="8" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="23" priority="8" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="containsText" dxfId="67" priority="7" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="22" priority="7" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="65" priority="5" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="64" priority="4" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",H19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="2" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",H19)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Value Entered" error="Valid values are between 1 and 1024 in int value" promptTitle="VHD Size Per User" prompt="Enter the VHD size in INT value, number must be between 1 and 1024" sqref="B10" xr:uid="{CBED2FD9-9304-492F-812B-63234547D67B}">
       <formula1>1</formula1>
       <formula2>1024</formula2>
@@ -5382,6 +5371,10 @@
       <formula2>168</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="VHD Size" prompt="Select the size of the user VHD defined in FSLogix Environment_x000a_" sqref="B7" xr:uid="{A1CCD0B8-6B2D-42A1-89B6-7ABA9C370E18}"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" errorTitle="IOPS: Incorrect Input" error="Please enter a whole number between 1 and 200." promptTitle="Storage IOPS: Env Dependant" prompt="Suggested values:_x000a_Per LoginVSI: 4_x000a_Per FSLogix Team: 15_x000a_With Offline Cache and Office365 Cache: 60 - 120" sqref="B4" xr:uid="{E2E3AE84-252F-4455-AC8B-A92442F4F96A}">
+      <formula1>1</formula1>
+      <formula2>200</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5401,18 +5394,12 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="If known, select the average storage I/O size.  If unknown, leave the value at the default of 32." promptTitle="Storage I/O Size (Advanced)" prompt="If known, select the average storage I/O size.  If unknown, leave the value at the default of 32." xr:uid="{86AD3042-EFBE-4769-8F55-A620876D83EA}">
           <x14:formula1>
             <xm:f>definitions!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>B8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Storage IOPS Per User" prompt="The average IOPS per user is environment dependant. " xr:uid="{E2E3AE84-252F-4455-AC8B-A92442F4F96A}">
-          <x14:formula1>
-            <xm:f>definitions!$B$2:$B$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Value Entered" error="Valid values are between 1 and 30  in int value" promptTitle="VHD Size Per User" prompt="Enter the VHD size in INT value, number must be between 1 and 1024" xr:uid="{F0468C29-122F-45A3-9E06-3D1D980A2EF8}">
           <x14:formula1>
@@ -5484,13 +5471,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="15"/>
     </row>
     <row r="2" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="15">
         <f>'FSLogix Calculator'!B$16</f>
@@ -5500,7 +5487,7 @@
     </row>
     <row r="3" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="15">
         <f>'FSLogix Calculator'!B$5</f>
@@ -5510,7 +5497,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="2">
         <f>_xlfn.XLOOKUP('FSLogix Calculator'!B$9,'Throughput Test'!G2:G12,'Throughput Test'!P$2:P$12)</f>
@@ -5520,7 +5507,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B5" s="2">
         <f>FLOOR(definitions!B24/'FSLogix Calculator'!B$5,1)</f>
@@ -5535,74 +5522,74 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="15">
         <f>('FSLogix Calculator'!B$13*1024)/definitions!B30</f>
         <v>3540</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="15">
         <f>('FSLogix Calculator'!B$13*1024)/definitions!B28</f>
         <v>885</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="15">
         <f>('FSLogix Calculator'!B$13*1024)/definitions!B26</f>
         <v>442.5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B11" s="2">
         <f>('FSLogix Calculator'!B$14*'FSLogix Calculator'!B$6)/definitions!B$30</f>
         <v>30</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="2">
         <f>('FSLogix Calculator'!B$14*'FSLogix Calculator'!B$6)/definitions!B28</f>
         <v>7.5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2">
         <f>('FSLogix Calculator'!B$14*'FSLogix Calculator'!B$6)/definitions!B26</f>
         <v>3.75</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5612,38 +5599,38 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="2">
         <f>CEILING(IF(B11&gt;B$3,definitions!B$31/B11,definitions!B$31/B$3),1)</f>
         <v>118</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="2">
         <f>CEILING(IF(B12&gt;B$3,definitions!B$31/B12,definitions!B$31/B$3),1)</f>
         <v>118</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2">
         <f>CEILING(IF(B13&gt;B$3,definitions!B$31/B13,definitions!B$31/B$3),1)</f>
         <v>118</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5653,38 +5640,38 @@
     </row>
     <row r="19" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="15" t="str">
         <f>IF(B$2&gt;B7,"Capacity","Bandwidth")</f>
         <v>Capacity</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="15" t="str">
         <f>IF(B$2&gt;B8,"Capacity","Bandwidth")</f>
         <v>Capacity</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="15" t="str">
         <f>IF(B$2&gt;B9,"Capacity","Bandwidth")</f>
         <v>Capacity</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5694,38 +5681,38 @@
     </row>
     <row r="23" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="15">
         <f>IF(B$2&gt;B7,B$2,B7)</f>
         <v>4130</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="15">
         <f>IF(B$2&gt;B8,B$2,B8)</f>
         <v>4130</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B25" s="15">
         <f>IF(B$2&gt;B9,B$2,B9)</f>
         <v>4130</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5735,38 +5722,38 @@
     </row>
     <row r="27" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" s="15" t="str">
         <f>IF(B23&gt;definitions!B$31,B19,"Capacity Pool Minimum Size")</f>
         <v>Capacity</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="15" t="str">
         <f>IF(B24&gt;definitions!B$31,B20,"Capacity Pool Minimum Size")</f>
         <v>Capacity</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29" s="15" t="str">
         <f>IF(B25&gt;definitions!B$31,B21,"Capacity Pool Minimum Size")</f>
         <v>Capacity</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5776,38 +5763,38 @@
     </row>
     <row r="31" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" s="15">
         <f>IF(B23&gt;definitions!B$31,B23,definitions!B$31)</f>
         <v>4130</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32" s="15">
         <f>IF(B24&gt;definitions!B$31,B24,definitions!B$31)</f>
         <v>4130</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" s="15">
         <f>IF(B25&gt;definitions!B$31,B25,definitions!B$31)</f>
         <v>4130</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5817,7 +5804,7 @@
     </row>
     <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B35" s="15" t="str">
         <f>IF(MIN(B31:B33)&gt;definitions!B24,"No","Yes")</f>
@@ -5827,7 +5814,7 @@
     </row>
     <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B36" s="2" t="str">
         <f>IF('FSLogix Calculator'!B3&gt;('FSLogix Calculator'!E24),"No","Yes")</f>
@@ -5846,42 +5833,42 @@
     </row>
     <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="24">
         <f>IF((B31&gt;definitions!B24),99999,B31*definitions!B$29)</f>
         <v>619.5</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="16">
         <f>IF((B32&gt;definitions!B24),99999,B32*definitions!B$27)</f>
         <v>1239</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="16">
         <f>IF((B33&gt;definitions!B24),99999,(B33*definitions!B$25))</f>
         <v>1652</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -5895,42 +5882,42 @@
     </row>
     <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" s="15">
         <f>B31/'FSLogix Calculator'!B$3</f>
         <v>35</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" s="15">
         <f>B32/'FSLogix Calculator'!B$3</f>
         <v>35</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" s="15">
         <f>B33/'FSLogix Calculator'!B$3</f>
         <v>35</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
@@ -5944,42 +5931,42 @@
     </row>
     <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="26">
         <f>IF(B38=definitions!A$23,B38, B38/'FSLogix Calculator'!B$29)</f>
         <v>1.4982876712328768</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="26">
         <f>IF(B39=definitions!A$23,B39, B39/'FSLogix Calculator'!B$29)</f>
         <v>2.9965753424657535</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="26">
         <f>IF(B40=definitions!A$23,B40, B40/'FSLogix Calculator'!B$29)</f>
         <v>3.9954337899543382</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
@@ -5992,46 +5979,46 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="26">
         <f>IF(B38=definitions!A23,B38,B38/'FSLogix Calculator'!B$37)</f>
         <v>0.6</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="26">
         <f>IF(B39=definitions!A23,B39,B39/'FSLogix Calculator'!B$37)</f>
         <v>1.2</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="26">
         <f>IF(B40=definitions!A23,B40,B40/'FSLogix Calculator'!B$37)</f>
         <v>1.6</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D52" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="77" t="s">
-        <v>107</v>
+      <c r="A54" s="76" t="s">
+        <v>106</v>
       </c>
       <c r="B54">
         <f>FLOOR(('Azure NetApp Files Calcuations'!B4*1024/'FSLogix Calculator'!B14)*(1/'FSLogix Calculator'!B6),1)</f>
@@ -6060,15 +6047,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="36" t="str">
         <f>IF('FSLogix Calculator'!B15&gt;definitions!B$38,"Required I/O rate exceeds documented 10,000 op rate upper limit","Yes")</f>
@@ -6081,7 +6068,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="38" t="str">
         <f>IF(('FSLogix Calculator'!B13)&gt;definitions!B$39,"Required bandwidth exceeds documented 300MiB/s  upper limit","Yes")</f>
@@ -6094,7 +6081,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="36" t="str">
         <f>IF('FSLogix Calculator'!B16&gt;102400,"Required capacity exceeds documented 100TiB upper limit","Yes")</f>
@@ -6107,7 +6094,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="37" t="str">
         <f>IF(('FSLogix Calculator'!B$4*'FSLogix Calculator'!B$3*'FSLogix Calculator'!B$6)&gt;definitions!B$40,"Required I/O rate exceeds documented 100,000 op rate upper limit","Yes")</f>
@@ -6120,7 +6107,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="37" t="str">
         <f>IF(IF(('FSLogix Calculator'!$B$4*'FSLogix Calculator'!$B$3*'FSLogix Calculator'!$B$6)&gt;('FSLogix Calculator'!$B$5*'FSLogix Calculator'!$B$3),'FSLogix Calculator'!$B$4*'FSLogix Calculator'!$B$3*'FSLogix Calculator'!$B$6,'FSLogix Calculator'!$B$5*'FSLogix Calculator'!$B$3)&gt;definitions!B42,"Required capacity exceeds documented 100TiB upper limit","Yes")</f>
@@ -6138,7 +6125,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="15">
         <f>(('FSLogix Calculator'!B13-('FSLogix Calculator'!B13*(1-'FSLogix Calculator'!B9)))-definitions!B43)/definitions!B44</f>
@@ -6147,7 +6134,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" s="15">
         <f>(('FSLogix Calculator'!B13-('FSLogix Calculator'!B13*'FSLogix Calculator'!B9))-definitions!B45)/definitions!B46</f>
@@ -6156,31 +6143,31 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" s="15">
         <f>IF(B8&lt;100,100,B8)</f>
         <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B11" s="15">
         <f>IF(B9&lt;100,100,B9)</f>
         <v>106.25</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B12" t="str">
         <f>_xlfn.XLOOKUP(MAX(B10:B11),B10:B11,C10:C11)</f>
@@ -6193,7 +6180,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B13" t="str">
         <f>IF(B9&gt;'FSLogix Calculator'!B3*'FSLogix Calculator'!B4*'FSLogix Calculator'!B6,"Bandwidth Need","I/O Need")</f>
@@ -6206,7 +6193,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B14" t="str">
         <f>IF(C13&gt;'FSLogix Calculator'!B16,'Azure Files Calculations'!B13,"Profile Size")</f>
@@ -6218,81 +6205,81 @@
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="75"/>
+      <c r="B17" s="74"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="75"/>
+      <c r="B18" s="74"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B4">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"No: 300MiB/s is Maximum Supported Load"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",B2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"""No: 102,400GiB is Maximum Supported Capacity"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>"No: 102,400GiB is Maximum Supported Capacity"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="No: Required ">
+    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="No: Required ">
       <formula>NOT(ISERROR(SEARCH("No: Required ",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C4">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="No:  Required ">
+    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="No:  Required ">
       <formula>NOT(ISERROR(SEARCH("No:  Required ",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="No:">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="No:">
       <formula>NOT(ISERROR(SEARCH("No:",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C6">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B6">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C6">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6324,13 +6311,13 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6489,23 +6476,23 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
         <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
       </c>
       <c r="D22" s="46"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B23" s="2"/>
       <c r="D23" s="46"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="15">
         <v>102400</v>
@@ -6514,7 +6501,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="24">
         <v>0.4</v>
@@ -6523,7 +6510,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="15">
         <v>128</v>
@@ -6532,7 +6519,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="24">
         <v>0.3</v>
@@ -6541,7 +6528,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="15">
         <v>64</v>
@@ -6550,7 +6537,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="24">
         <v>0.15</v>
@@ -6559,7 +6546,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="15">
         <v>16</v>
@@ -6568,7 +6555,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="15">
         <v>4096</v>
@@ -6586,7 +6573,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B33" s="15">
         <v>12</v>
@@ -6603,7 +6590,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" s="24">
         <v>0.06</v>
@@ -6612,7 +6599,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" s="25">
         <f>0.0015/10000</f>
@@ -6621,7 +6608,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B37" s="24">
         <v>0.25</v>
@@ -6629,7 +6616,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B38" s="15">
         <v>10000</v>
@@ -6637,7 +6624,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B39" s="15">
         <v>300</v>
@@ -6645,7 +6632,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B40" s="15">
         <v>100000</v>
@@ -6653,7 +6640,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B41" s="15">
         <v>102400</v>
@@ -6661,7 +6648,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" s="15">
         <v>102400</v>
@@ -6669,7 +6656,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B43" s="15">
         <v>60</v>
@@ -6677,15 +6664,15 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="B44" s="74">
+        <v>157</v>
+      </c>
+      <c r="B44" s="73">
         <v>0.06</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B45" s="15">
         <v>40</v>
@@ -6693,15 +6680,15 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>160</v>
-      </c>
-      <c r="B46" s="74">
+        <v>159</v>
+      </c>
+      <c r="B46" s="73">
         <v>0.04</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B47" s="26">
         <v>0.4</v>
@@ -6721,7 +6708,7 @@
   <dimension ref="A1:AI12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R16"/>
+      <selection activeCell="G2" sqref="G2:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6736,120 +6723,120 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
         <v>128</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>129</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>130</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>131</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>132</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>133</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>134</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>135</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>136</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>137</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>138</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>139</v>
       </c>
-      <c r="M1" t="s">
-        <v>140</v>
-      </c>
       <c r="N1" t="s">
+        <v>129</v>
+      </c>
+      <c r="O1" t="s">
         <v>130</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>131</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>132</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>133</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>134</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>135</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>136</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>137</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>138</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>139</v>
       </c>
-      <c r="X1" t="s">
-        <v>140</v>
-      </c>
       <c r="Y1" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z1" t="s">
         <v>130</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>131</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>132</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>133</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>134</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>135</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>136</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>137</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>138</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>139</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
         <v>114</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>115</v>
-      </c>
-      <c r="C2" t="s">
-        <v>116</v>
       </c>
       <c r="D2">
         <v>9027</v>
@@ -6882,7 +6869,7 @@
         <v>124</v>
       </c>
       <c r="N2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O2">
         <v>60267</v>
@@ -6894,7 +6881,7 @@
         <v>65536</v>
       </c>
       <c r="R2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S2">
         <v>2.1063333333299998</v>
@@ -6915,7 +6902,7 @@
         <v>126</v>
       </c>
       <c r="Y2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z2">
         <v>17027</v>
@@ -6927,7 +6914,7 @@
         <v>65536</v>
       </c>
       <c r="AC2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AD2">
         <v>7.4829999999999997</v>
@@ -6950,13 +6937,13 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
         <v>114</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>115</v>
-      </c>
-      <c r="C3" t="s">
-        <v>116</v>
       </c>
       <c r="D3">
         <v>8997</v>
@@ -6989,7 +6976,7 @@
         <v>125</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O3">
         <v>57317</v>
@@ -7001,7 +6988,7 @@
         <v>65536</v>
       </c>
       <c r="R3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S3">
         <v>2.2126666666700001</v>
@@ -7022,7 +7009,7 @@
         <v>126</v>
       </c>
       <c r="Y3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z3">
         <v>18481</v>
@@ -7034,7 +7021,7 @@
         <v>65536</v>
       </c>
       <c r="AC3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AD3">
         <v>6.8860000000000001</v>
@@ -7057,13 +7044,13 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
         <v>114</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>115</v>
-      </c>
-      <c r="C4" t="s">
-        <v>116</v>
       </c>
       <c r="D4">
         <v>8570</v>
@@ -7096,7 +7083,7 @@
         <v>125</v>
       </c>
       <c r="N4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O4">
         <v>52732</v>
@@ -7108,7 +7095,7 @@
         <v>65536</v>
       </c>
       <c r="R4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S4">
         <v>2.4056666666700002</v>
@@ -7129,7 +7116,7 @@
         <v>126</v>
       </c>
       <c r="Y4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z4">
         <v>19153</v>
@@ -7141,7 +7128,7 @@
         <v>65536</v>
       </c>
       <c r="AC4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD4">
         <v>6.6449999999999996</v>
@@ -7164,13 +7151,13 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
         <v>114</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>115</v>
-      </c>
-      <c r="C5" t="s">
-        <v>116</v>
       </c>
       <c r="D5">
         <v>7871</v>
@@ -7203,7 +7190,7 @@
         <v>125</v>
       </c>
       <c r="N5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O5">
         <v>51478</v>
@@ -7215,7 +7202,7 @@
         <v>65536</v>
       </c>
       <c r="R5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S5">
         <v>2.4623333333300002</v>
@@ -7236,7 +7223,7 @@
         <v>126</v>
       </c>
       <c r="Y5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z5">
         <v>19764</v>
@@ -7248,7 +7235,7 @@
         <v>65536</v>
       </c>
       <c r="AC5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AD5">
         <v>6.4393333333299996</v>
@@ -7271,13 +7258,13 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
         <v>114</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>115</v>
-      </c>
-      <c r="C6" t="s">
-        <v>116</v>
       </c>
       <c r="D6">
         <v>6853</v>
@@ -7310,7 +7297,7 @@
         <v>124</v>
       </c>
       <c r="N6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O6">
         <v>48993</v>
@@ -7322,7 +7309,7 @@
         <v>65536</v>
       </c>
       <c r="R6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S6">
         <v>2.5903333333299998</v>
@@ -7343,7 +7330,7 @@
         <v>126</v>
       </c>
       <c r="Y6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z6">
         <v>19712</v>
@@ -7355,7 +7342,7 @@
         <v>65536</v>
       </c>
       <c r="AC6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD6">
         <v>6.4546666666699997</v>
@@ -7378,13 +7365,13 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" t="s">
         <v>114</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>115</v>
-      </c>
-      <c r="C7" t="s">
-        <v>116</v>
       </c>
       <c r="D7">
         <v>9303</v>
@@ -7417,7 +7404,7 @@
         <v>123</v>
       </c>
       <c r="N7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O7">
         <v>47054</v>
@@ -7429,7 +7416,7 @@
         <v>65536</v>
       </c>
       <c r="R7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S7">
         <v>2.6956666666700002</v>
@@ -7450,7 +7437,7 @@
         <v>126</v>
       </c>
       <c r="Y7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z7">
         <v>19788</v>
@@ -7462,7 +7449,7 @@
         <v>65536</v>
       </c>
       <c r="AC7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AD7">
         <v>6.4283333333300003</v>
@@ -7485,13 +7472,13 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
         <v>114</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>115</v>
-      </c>
-      <c r="C8" t="s">
-        <v>116</v>
       </c>
       <c r="D8">
         <v>7216</v>
@@ -7524,7 +7511,7 @@
         <v>125</v>
       </c>
       <c r="N8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O8">
         <v>42934</v>
@@ -7536,7 +7523,7 @@
         <v>65536</v>
       </c>
       <c r="R8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S8">
         <v>2.9540000000000002</v>
@@ -7557,7 +7544,7 @@
         <v>126</v>
       </c>
       <c r="Y8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z8">
         <v>18790</v>
@@ -7569,7 +7556,7 @@
         <v>65536</v>
       </c>
       <c r="AC8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AD8">
         <v>6.7686666666699997</v>
@@ -7592,13 +7579,13 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" t="s">
         <v>114</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>115</v>
-      </c>
-      <c r="C9" t="s">
-        <v>116</v>
       </c>
       <c r="D9">
         <v>8643</v>
@@ -7631,7 +7618,7 @@
         <v>125</v>
       </c>
       <c r="N9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O9">
         <v>38865</v>
@@ -7643,7 +7630,7 @@
         <v>65536</v>
       </c>
       <c r="R9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S9">
         <v>3.26633333333</v>
@@ -7664,7 +7651,7 @@
         <v>126</v>
       </c>
       <c r="Y9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z9">
         <v>17559</v>
@@ -7676,7 +7663,7 @@
         <v>65536</v>
       </c>
       <c r="AC9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AD9">
         <v>7.2423333333300004</v>
@@ -7699,13 +7686,13 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" t="s">
         <v>114</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>115</v>
-      </c>
-      <c r="C10" t="s">
-        <v>116</v>
       </c>
       <c r="D10">
         <v>8431</v>
@@ -7738,7 +7725,7 @@
         <v>126</v>
       </c>
       <c r="N10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O10">
         <v>35170</v>
@@ -7750,7 +7737,7 @@
         <v>65536</v>
       </c>
       <c r="R10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S10">
         <v>3.6153333333300002</v>
@@ -7771,7 +7758,7 @@
         <v>126</v>
       </c>
       <c r="Y10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z10">
         <v>16162</v>
@@ -7783,7 +7770,7 @@
         <v>65536</v>
       </c>
       <c r="AC10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AD10">
         <v>7.8673333333300004</v>
@@ -7806,13 +7793,13 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
         <v>114</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>115</v>
-      </c>
-      <c r="C11" t="s">
-        <v>116</v>
       </c>
       <c r="D11">
         <v>10134</v>
@@ -7845,7 +7832,7 @@
         <v>125</v>
       </c>
       <c r="N11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O11">
         <v>31849</v>
@@ -7857,7 +7844,7 @@
         <v>65536</v>
       </c>
       <c r="R11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S11">
         <v>3.99633333333</v>
@@ -7878,7 +7865,7 @@
         <v>126</v>
       </c>
       <c r="Y11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z11">
         <v>15215</v>
@@ -7890,7 +7877,7 @@
         <v>65536</v>
       </c>
       <c r="AC11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AD11">
         <v>8.3573333333300006</v>
@@ -7913,13 +7900,13 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s">
         <v>114</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>115</v>
-      </c>
-      <c r="C12" t="s">
-        <v>116</v>
       </c>
       <c r="D12">
         <v>9700</v>
@@ -7952,7 +7939,7 @@
         <v>127</v>
       </c>
       <c r="N12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O12">
         <v>29482</v>
@@ -7964,7 +7951,7 @@
         <v>65536</v>
       </c>
       <c r="R12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="S12">
         <v>4.3016666666700001</v>
@@ -7985,7 +7972,7 @@
         <v>126</v>
       </c>
       <c r="Y12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Z12">
         <v>14265</v>
@@ -7997,7 +7984,7 @@
         <v>65536</v>
       </c>
       <c r="AC12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AD12">
         <v>8.9133333333299998</v>
@@ -8031,15 +8018,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100050FBA8A9F0AFB4BB2D0148D6A234C38" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74183e733b66e5e9a3cd5553bd4bd9ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4a052287-e6d5-446a-afc6-58987b850d5f" xmlns:ns4="943a090e-7b96-4eb7-abc0-264fa36c6c5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b903754823e47922d1d3c75b6236d24" ns3:_="" ns4:_="">
     <xsd:import namespace="4a052287-e6d5-446a-afc6-58987b850d5f"/>
@@ -8262,6 +8240,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7769B51B-49EA-4054-A0C2-A13FF67FB754}">
   <ds:schemaRefs>
@@ -8280,14 +8267,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEC18BF-42E1-4B07-B0F9-328B1505E1A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{097D0541-97F4-46BE-8711-51CFA8DE5931}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8304,4 +8283,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEC18BF-42E1-4B07-B0F9-328B1505E1A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Removed Link To Foreign File
</commit_message>
<xml_diff>
--- a/fslogix-storage-calculator.xlsx
+++ b/fslogix-storage-calculator.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netapp-my.sharepoint.com/personal/mchad_netapp_com/Documents/Documents/DataFabric/calculators/fslogix-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{80057BE8-5265-429A-8C17-C870DB06A720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{139D8C4D-F01E-4B3F-83D6-81314EE328FE}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="t+JkNq9tqmsPWKZG4243dmROwKF3bq/0/pMp0U7P3IbsgB19gsMVOhnXvXvDRyuLi2nqOQxBUhOjuGiZBOrHlQ==" workbookSaltValue="OSy8GVs1Yity0kiwcucv5A==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{80057BE8-5265-429A-8C17-C870DB06A720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EEBFEAFB-EFFE-4838-B7E1-BCA353958299}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{CB3913B2-BB8F-4CB3-9459-2FD527F7F31B}"/>
   </bookViews>
@@ -17,12 +16,9 @@
     <sheet name="FSLogix Calculator" sheetId="1" r:id="rId1"/>
     <sheet name="Azure NetApp Files Calcuations" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="Azure Files Calculations" sheetId="4" state="hidden" r:id="rId3"/>
-    <sheet name="definitions" sheetId="2" state="hidden" r:id="rId4"/>
-    <sheet name="Throughput Test" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="definitions" sheetId="2" r:id="rId4"/>
+    <sheet name="Throughput Test" sheetId="5" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="191029" iterate="1" iterateCount="3"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -934,6 +930,21 @@
   </cellStyles>
   <dxfs count="98">
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1092,349 +1103,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1762,6 +1430,334 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1885,13 +1881,18 @@
           <c:cat>
             <c:strRef>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'[1]VDBENCH APF|AF|ANF'!$G$2:$G$12</c15:sqref>
-                  </c15:fullRef>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="2">
+                        <c:v>Readpct=80</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c16:filteredLitCache>
                 </c:ext>
               </c:extLst>
-              <c:f>('[1]VDBENCH APF|AF|ANF'!$G$2:$G$3,'[1]VDBENCH APF|AF|ANF'!$G$5:$G$12)</c:f>
+              <c:f/>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1930,13 +1931,19 @@
           <c:val>
             <c:numRef>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'[1]VDBENCH APF|AF|ANF'!$E$145:$E$155</c15:sqref>
-                  </c15:fullRef>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="2">
+                        <c:v>535</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c16:filteredLitCache>
                 </c:ext>
               </c:extLst>
-              <c:f>('[1]VDBENCH APF|AF|ANF'!$E$145:$E$146,'[1]VDBENCH APF|AF|ANF'!$E$148:$E$155)</c:f>
+              <c:f/>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2038,13 +2045,19 @@
           <c:val>
             <c:numRef>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'[1]VDBENCH APF|AF|ANF'!$P$145:$P$155</c15:sqref>
-                  </c15:fullRef>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="2">
+                        <c:v>3295</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c16:filteredLitCache>
                 </c:ext>
               </c:extLst>
-              <c:f>('[1]VDBENCH APF|AF|ANF'!$P$145:$P$146,'[1]VDBENCH APF|AF|ANF'!$P$148:$P$155)</c:f>
+              <c:f/>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2146,13 +2159,19 @@
           <c:val>
             <c:numRef>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'[1]VDBENCH APF|AF|ANF'!$AA$145:$AA$155</c15:sqref>
-                  </c15:fullRef>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="2">
+                        <c:v>1197</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c16:filteredLitCache>
                 </c:ext>
               </c:extLst>
-              <c:f>('[1]VDBENCH APF|AF|ANF'!$AA$145:$AA$146,'[1]VDBENCH APF|AF|ANF'!$AA$148:$AA$155)</c:f>
+              <c:f/>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2271,13 +2290,19 @@
           <c:val>
             <c:numRef>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'[1]VDBENCH APF|AF|ANF'!$H$145:$H$155</c15:sqref>
-                  </c15:fullRef>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="2">
+                        <c:v>14.6566666667</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c16:filteredLitCache>
                 </c:ext>
               </c:extLst>
-              <c:f>('[1]VDBENCH APF|AF|ANF'!$H$145:$H$146,'[1]VDBENCH APF|AF|ANF'!$H$148:$H$155)</c:f>
+              <c:f/>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2382,13 +2407,19 @@
           <c:val>
             <c:numRef>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'[1]VDBENCH APF|AF|ANF'!$S$145:$S$155</c15:sqref>
-                  </c15:fullRef>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="2">
+                        <c:v>2.4056666666700002</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c16:filteredLitCache>
                 </c:ext>
               </c:extLst>
-              <c:f>('[1]VDBENCH APF|AF|ANF'!$S$145:$S$146,'[1]VDBENCH APF|AF|ANF'!$S$148:$S$155)</c:f>
+              <c:f/>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2493,13 +2524,19 @@
           <c:val>
             <c:numRef>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'[1]VDBENCH APF|AF|ANF'!$AD$145:$AD$155</c15:sqref>
-                  </c15:fullRef>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{F5D05F6E-A05E-4728-AFD3-386EB277150F}">
+                  <c16:filteredLitCache>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="2">
+                        <c:v>6.6449999999999996</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c16:filteredLitCache>
                 </c:ext>
               </c:extLst>
-              <c:f>('[1]VDBENCH APF|AF|ANF'!$AD$145:$AD$146,'[1]VDBENCH APF|AF|ANF'!$AD$148:$AD$155)</c:f>
+              <c:f/>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -3572,413 +3609,85 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="(1)FirstLogin50usersAF(d32)"/>
-      <sheetName val="login script"/>
-      <sheetName val="(1)FirstLogin50usersANF(d16sv3)"/>
-      <sheetName val="(2)FirstLogin50usersANF(d16sv3)"/>
-      <sheetName val="(1)FirstLogin50usersANF(d32)"/>
-      <sheetName val="(1)FirstLogin50usersANFd1984GP"/>
-      <sheetName val="(1)2ndLogin50usersANF(d32)"/>
-      <sheetName val="(2)2ndLogin50usersANF(d32)"/>
-      <sheetName val="ANF|APF|AF Powerpoint"/>
-      <sheetName val="VDBENCH APF|AF|ANF"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="VDBENCH APF|ANF"/>
-      <sheetName val="VDBENCH ANF|ANF"/>
-      <sheetName val="VDBENCH APF|AF"/>
-      <sheetName val="VDBENCH APF|APF"/>
-      <sheetName val="VDBENCH AF|AF"/>
-      <sheetName val="Evidence of Object Storage AF"/>
-      <sheetName val="APF Cost Per MiBs"/>
-      <sheetName val="RogersRealWorld_vol_stats"/>
-      <sheetName val="RogersRealWorld_workload_stats"/>
-      <sheetName val="Sheet4"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="9">
-        <row r="2">
-          <cell r="G2" t="str">
-            <v>Readpct=100</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="G3" t="str">
-            <v>Readpct=90</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="G4" t="str">
-            <v>Readpct=80</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="G5" t="str">
-            <v>Readpct=70</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="G6" t="str">
-            <v>Readpct=60</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="G7" t="str">
-            <v>Readpct=50</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="G8" t="str">
-            <v>Readpct=40</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="G9" t="str">
-            <v>Readpct=30</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="G10" t="str">
-            <v>Readpct=20</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="G11" t="str">
-            <v>Readpct=10</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="G12" t="str">
-            <v>Readpct=0</v>
-          </cell>
-        </row>
-        <row r="145">
-          <cell r="E145">
-            <v>564</v>
-          </cell>
-          <cell r="H145">
-            <v>13.820666666699999</v>
-          </cell>
-          <cell r="P145">
-            <v>3766</v>
-          </cell>
-          <cell r="S145">
-            <v>2.1063333333299998</v>
-          </cell>
-          <cell r="AA145">
-            <v>1064</v>
-          </cell>
-          <cell r="AD145">
-            <v>7.4829999999999997</v>
-          </cell>
-        </row>
-        <row r="146">
-          <cell r="E146">
-            <v>562</v>
-          </cell>
-          <cell r="H146">
-            <v>13.823</v>
-          </cell>
-          <cell r="P146">
-            <v>3582</v>
-          </cell>
-          <cell r="S146">
-            <v>2.2126666666700001</v>
-          </cell>
-          <cell r="AA146">
-            <v>1155</v>
-          </cell>
-          <cell r="AD146">
-            <v>6.8860000000000001</v>
-          </cell>
-        </row>
-        <row r="147">
-          <cell r="E147">
-            <v>535</v>
-          </cell>
-          <cell r="H147">
-            <v>14.6566666667</v>
-          </cell>
-          <cell r="P147">
-            <v>3295</v>
-          </cell>
-          <cell r="S147">
-            <v>2.4056666666700002</v>
-          </cell>
-          <cell r="AA147">
-            <v>1197</v>
-          </cell>
-          <cell r="AD147">
-            <v>6.6449999999999996</v>
-          </cell>
-        </row>
-        <row r="148">
-          <cell r="E148">
-            <v>491</v>
-          </cell>
-          <cell r="H148">
-            <v>15.9073333333</v>
-          </cell>
-          <cell r="P148">
-            <v>3217</v>
-          </cell>
-          <cell r="S148">
-            <v>2.4623333333300002</v>
-          </cell>
-          <cell r="AA148">
-            <v>1235</v>
-          </cell>
-          <cell r="AD148">
-            <v>6.4393333333299996</v>
-          </cell>
-        </row>
-        <row r="149">
-          <cell r="E149">
-            <v>428</v>
-          </cell>
-          <cell r="H149">
-            <v>18.195666666699999</v>
-          </cell>
-          <cell r="P149">
-            <v>3062</v>
-          </cell>
-          <cell r="S149">
-            <v>2.5903333333299998</v>
-          </cell>
-          <cell r="AA149">
-            <v>1232</v>
-          </cell>
-          <cell r="AD149">
-            <v>6.4546666666699997</v>
-          </cell>
-        </row>
-        <row r="150">
-          <cell r="E150">
-            <v>581</v>
-          </cell>
-          <cell r="H150">
-            <v>13.262666666699999</v>
-          </cell>
-          <cell r="P150">
-            <v>2940</v>
-          </cell>
-          <cell r="S150">
-            <v>2.6956666666700002</v>
-          </cell>
-          <cell r="AA150">
-            <v>1236</v>
-          </cell>
-          <cell r="AD150">
-            <v>6.4283333333300003</v>
-          </cell>
-        </row>
-        <row r="151">
-          <cell r="E151">
-            <v>451</v>
-          </cell>
-          <cell r="H151">
-            <v>17.063666666700001</v>
-          </cell>
-          <cell r="P151">
-            <v>2683</v>
-          </cell>
-          <cell r="S151">
-            <v>2.9540000000000002</v>
-          </cell>
-          <cell r="AA151">
-            <v>1174</v>
-          </cell>
-          <cell r="AD151">
-            <v>6.7686666666699997</v>
-          </cell>
-        </row>
-        <row r="152">
-          <cell r="E152">
-            <v>540</v>
-          </cell>
-          <cell r="H152">
-            <v>14.683999999999999</v>
-          </cell>
-          <cell r="P152">
-            <v>2429</v>
-          </cell>
-          <cell r="S152">
-            <v>3.26633333333</v>
-          </cell>
-          <cell r="AA152">
-            <v>1097</v>
-          </cell>
-          <cell r="AD152">
-            <v>7.2423333333300004</v>
-          </cell>
-        </row>
-        <row r="153">
-          <cell r="E153">
-            <v>526</v>
-          </cell>
-          <cell r="H153">
-            <v>15.0756666667</v>
-          </cell>
-          <cell r="P153">
-            <v>2198</v>
-          </cell>
-          <cell r="S153">
-            <v>3.6153333333300002</v>
-          </cell>
-          <cell r="AA153">
-            <v>1010</v>
-          </cell>
-          <cell r="AD153">
-            <v>7.8673333333300004</v>
-          </cell>
-        </row>
-        <row r="154">
-          <cell r="E154">
-            <v>633</v>
-          </cell>
-          <cell r="H154">
-            <v>12.279666666700001</v>
-          </cell>
-          <cell r="P154">
-            <v>1990</v>
-          </cell>
-          <cell r="S154">
-            <v>3.99633333333</v>
-          </cell>
-          <cell r="AA154">
-            <v>950</v>
-          </cell>
-          <cell r="AD154">
-            <v>8.3573333333300006</v>
-          </cell>
-        </row>
-        <row r="155">
-          <cell r="E155">
-            <v>606</v>
-          </cell>
-          <cell r="H155">
-            <v>13.119666666700001</v>
-          </cell>
-          <cell r="P155">
-            <v>1842</v>
-          </cell>
-          <cell r="S155">
-            <v>4.3016666666700001</v>
-          </cell>
-          <cell r="AA155">
-            <v>891</v>
-          </cell>
-          <cell r="AD155">
-            <v>8.9133333333299998</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{856F6794-4173-4194-B8E4-7BB540367D16}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96" tableBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{856F6794-4173-4194-B8E4-7BB540367D16}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
   <autoFilter ref="A2:B9" xr:uid="{91E6A135-C0E7-4D0B-8EB4-141892DA45C5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2F564818-5A0F-4075-8D5E-BCEC57D8FC3C}" name="Fields" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{D42113E7-14D7-4A36-BB89-433CD657FB9D}" name="Input " dataDxfId="93"/>
+    <tableColumn id="1" xr3:uid="{2F564818-5A0F-4075-8D5E-BCEC57D8FC3C}" name="Fields" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{D42113E7-14D7-4A36-BB89-433CD657FB9D}" name="Input " dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5554924-003B-4661-B33F-97EE2DB8E4A1}" name="Table8" displayName="Table8" ref="A22:B47" totalsRowShown="0" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5554924-003B-4661-B33F-97EE2DB8E4A1}" name="Table8" displayName="Table8" ref="A22:B47" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="A22:B47" xr:uid="{783E58C8-C7D9-4121-86C6-A6F7E49A97E3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{62872274-DD35-4869-BA93-32B33621B006}" name="Keys" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{BCBEE816-C2FF-4BB7-8812-71E8D95CE734}" name="Values" dataDxfId="53"/>
+    <tableColumn id="1" xr3:uid="{62872274-DD35-4869-BA93-32B33621B006}" name="Keys" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{BCBEE816-C2FF-4BB7-8812-71E8D95CE734}" name="Values" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E152E804-6E16-4FE5-822A-359F4049D3B1}" name="Table2" displayName="Table2" ref="A28:B32" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91" tableBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E152E804-6E16-4FE5-822A-359F4049D3B1}" name="Table2" displayName="Table2" ref="A28:B32" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
   <autoFilter ref="A28:B32" xr:uid="{4897B486-AB3B-4450-B296-0E35971B3AE2}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3A7044B6-6E00-4BEF-9FE6-A7DEE00EE3F3}" name="Azure Files Price Break Down" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{6BB28A88-2884-4CC5-80B3-4CA3051CCAC3}" name="Calculated Output" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{3A7044B6-6E00-4BEF-9FE6-A7DEE00EE3F3}" name="Azure Files Price Break Down" dataDxfId="52"/>
+    <tableColumn id="2" xr3:uid="{6BB28A88-2884-4CC5-80B3-4CA3051CCAC3}" name="Calculated Output" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BA317605-A8C7-4DFA-9894-A955BD37C1CF}" name="Table4" displayName="Table4" ref="A11:B16" totalsRowShown="0" headerRowDxfId="87" tableBorderDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BA317605-A8C7-4DFA-9894-A955BD37C1CF}" name="Table4" displayName="Table4" ref="A11:B16" totalsRowShown="0" headerRowDxfId="50" tableBorderDxfId="49">
   <autoFilter ref="A11:B16" xr:uid="{FDD62D26-CF49-4DB8-BB86-E5640AFB3072}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{98F6AE4C-A8FE-46A2-B695-4F7EC29B79C1}" name="High Level Environmental Needs" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{923448D6-8587-46CF-AC83-4786C0E6E31A}" name="Calculated Output" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{98F6AE4C-A8FE-46A2-B695-4F7EC29B79C1}" name="High Level Environmental Needs" dataDxfId="48"/>
+    <tableColumn id="2" xr3:uid="{923448D6-8587-46CF-AC83-4786C0E6E31A}" name="Calculated Output" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E9B81EED-ACF0-4F74-94BF-2331D9B58AEF}" name="Table5" displayName="Table5" ref="A36:B38" totalsRowShown="0" dataDxfId="83" tableBorderDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E9B81EED-ACF0-4F74-94BF-2331D9B58AEF}" name="Table5" displayName="Table5" ref="A36:B38" totalsRowShown="0" dataDxfId="46" tableBorderDxfId="45">
   <autoFilter ref="A36:B38" xr:uid="{F64951B7-0541-475C-8E4E-15CB609631E0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EEA382B5-FB82-4F1D-9327-A87385C52897}" name="Azure Premium Files Price Break Down" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{E770553C-A0C0-45E6-BC23-3E0DD3249B14}" name="Calculated Output" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{EEA382B5-FB82-4F1D-9327-A87385C52897}" name="Azure Premium Files Price Break Down" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{E770553C-A0C0-45E6-BC23-3E0DD3249B14}" name="Calculated Output" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{72039F74-6304-436F-9B2C-E726744D9970}" name="Table9" displayName="Table9" ref="A18:B22" totalsRowShown="0" dataDxfId="79" tableBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{72039F74-6304-436F-9B2C-E726744D9970}" name="Table9" displayName="Table9" ref="A18:B22" totalsRowShown="0" dataDxfId="42" tableBorderDxfId="41">
   <autoFilter ref="A18:B22" xr:uid="{1849FF8B-C5DF-48B3-BD49-7E1B6D720287}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3F78E685-9C28-44F6-9A2A-3F9135F54C28}" name="Azure NetApp Files Price Break Down" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{AA370671-CA18-4101-A4C3-7BC422CCC1F1}" name="Calculated Output" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{3F78E685-9C28-44F6-9A2A-3F9135F54C28}" name="Azure NetApp Files Price Break Down" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{AA370671-CA18-4101-A4C3-7BC422CCC1F1}" name="Calculated Output" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{2F4EE936-97FF-430B-BCE0-3BA4433FF3D4}" name="Table91119" displayName="Table91119" ref="D18:H26" totalsRowShown="0" dataDxfId="75" tableBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{2F4EE936-97FF-430B-BCE0-3BA4433FF3D4}" name="Table91119" displayName="Table91119" ref="D18:H26" totalsRowShown="0" dataDxfId="38" tableBorderDxfId="37">
   <autoFilter ref="D18:H26" xr:uid="{F75E429C-8018-41C4-B4C3-C0AD783F2D38}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{25D43E32-76CE-4E57-9637-4A7FD2463E37}" name="Azure NetApp Files Additional Information" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{3C9CF5B6-EAB8-4222-9C96-5A10EE28F85F}" name=" Output" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{F8FAE1CB-5733-4CC5-9F68-AD29EB511AF6}" name="Etc(1)" dataDxfId="70">
+    <tableColumn id="1" xr3:uid="{25D43E32-76CE-4E57-9637-4A7FD2463E37}" name="Azure NetApp Files Additional Information" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{3C9CF5B6-EAB8-4222-9C96-5A10EE28F85F}" name=" Output" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{F8FAE1CB-5733-4CC5-9F68-AD29EB511AF6}" name="Etc(1)" dataDxfId="33">
       <calculatedColumnFormula>IF(E20&gt;definitions!B24,definitions!$A$23,"Yes")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2A8935D0-2756-4A0D-B01F-87C8DFAE1AD5}" name="Etc(2)" dataDxfId="69">
+    <tableColumn id="4" xr3:uid="{2A8935D0-2756-4A0D-B01F-87C8DFAE1AD5}" name="Etc(2)" dataDxfId="32">
       <calculatedColumnFormula>IF(B3&gt;E24,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7CD54AC1-822B-4FE1-B7D3-C9A779DEF8FC}" name="Etc(3)" dataDxfId="68">
+    <tableColumn id="5" xr3:uid="{7CD54AC1-822B-4FE1-B7D3-C9A779DEF8FC}" name="Etc(3)" dataDxfId="31">
       <calculatedColumnFormula>IF(B3&gt;E24,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3987,18 +3696,18 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{E617B910-6016-4284-B1B7-B2BDBB2DAC94}" name="Table622" displayName="Table622" ref="D28:H34" totalsRowShown="0" headerRowDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{E617B910-6016-4284-B1B7-B2BDBB2DAC94}" name="Table622" displayName="Table622" ref="D28:H34" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="D28:H34" xr:uid="{6432D5DC-E020-4F4A-81F0-AFAE2FFBB2FE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{284AB7F5-C1F5-4923-8D18-8B326F2B7795}" name="Azure Standard Files Additional Information"/>
-    <tableColumn id="2" xr3:uid="{A95529E7-EF42-4D6F-BDD9-4D129864E797}" name="Output" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{9881ABB1-4E08-4030-AEC9-CCA810605C29}" name="Etc(1)" dataDxfId="64">
+    <tableColumn id="2" xr3:uid="{A95529E7-EF42-4D6F-BDD9-4D129864E797}" name="Output" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{9881ABB1-4E08-4030-AEC9-CCA810605C29}" name="Etc(1)" dataDxfId="27">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5BC3DEF6-CDB9-4DE9-B8FF-9749CBA220CD}" name="Etc(2)" dataDxfId="63">
+    <tableColumn id="4" xr3:uid="{5BC3DEF6-CDB9-4DE9-B8FF-9749CBA220CD}" name="Etc(2)" dataDxfId="26">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3F802064-6239-4D79-9EEF-E6B1422584F4}" name="Etc(3)" dataDxfId="62">
+    <tableColumn id="5" xr3:uid="{3F802064-6239-4D79-9EEF-E6B1422584F4}" name="Etc(3)" dataDxfId="25">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4007,15 +3716,15 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{017E12BE-FEED-449C-A993-3E3DA447FC83}" name="Table61423" displayName="Table61423" ref="D36:G42" totalsRowShown="0" headerRowDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{017E12BE-FEED-449C-A993-3E3DA447FC83}" name="Table61423" displayName="Table61423" ref="D36:G42" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="D36:G42" xr:uid="{35197520-871D-45A1-92D2-3E64562C597C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7454E181-1F78-43D7-992D-393BF7E62908}" name="Azure Premium Files Additional Information"/>
-    <tableColumn id="2" xr3:uid="{D283543A-6DF3-46B8-B880-680345E5383E}" name="output" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{383E5A06-7313-4E3D-A474-C65E865DB16D}" name="Etc(1)" dataDxfId="58">
+    <tableColumn id="2" xr3:uid="{D283543A-6DF3-46B8-B880-680345E5383E}" name="output" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{383E5A06-7313-4E3D-A474-C65E865DB16D}" name="Etc(1)" dataDxfId="21">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{22B7B0DB-CD46-43E2-A4B8-192176C63B53}" name="Etc(2)" dataDxfId="57">
+    <tableColumn id="4" xr3:uid="{22B7B0DB-CD46-43E2-A4B8-192176C63B53}" name="Etc(2)" dataDxfId="20">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4030,7 +3739,7 @@
     <tableColumn id="2" xr3:uid="{9191646A-D382-43C8-AD5D-D9379A6352B8}" name="IO Size"/>
     <tableColumn id="3" xr3:uid="{B94E1025-3714-4DA4-824F-A38F565F77F4}" name="IOPS Per User"/>
     <tableColumn id="1" xr3:uid="{E67A9471-95D1-42FF-B18E-7D012DE67FD4}" name="VHD Sizes"/>
-    <tableColumn id="4" xr3:uid="{779397D8-86EA-41AE-9217-A6D49A13139B}" name="Concurrent Users" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{779397D8-86EA-41AE-9217-A6D49A13139B}" name="Concurrent Users" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{5EBEBC80-5940-4420-B7CB-91D5FC7DF075}" name="Read Percenage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4340,7 +4049,7 @@
   <dimension ref="A1:H112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5193,163 +4902,163 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A36:B39 A28:B34">
-    <cfRule type="cellIs" dxfId="52" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="93" operator="equal">
       <formula>"Temporarily Empty Field"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:H31">
-    <cfRule type="containsText" dxfId="51" priority="23" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="96" priority="23" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="24" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="95" priority="24" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",F29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E23">
-    <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="41" operator="equal">
       <formula>"Capacity Pool Minimum Size"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="48" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="40" operator="equal">
       <formula>"Temporarily Empty Field"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="47" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="39" operator="equal">
       <formula>"Temporarily Empty Field"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="46" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="31" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="32" operator="equal">
       <formula>"""Yes"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="38" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="33" operator="equal">
       <formula>"Required Capacity Exceeds documented 100TiB Upper Limit"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="34" operator="equal">
       <formula>"""Required Capacity Exceeds documented 100TiB Upper Limit"""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="35" operator="containsText" text="&quot;Required&quot;">
+    <cfRule type="containsText" dxfId="86" priority="35" operator="containsText" text="&quot;Required&quot;">
       <formula>NOT(ISERROR(SEARCH("""Required""",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="36" operator="containsText" text="&quot;Required&quot;">
+    <cfRule type="containsText" dxfId="85" priority="36" operator="containsText" text="&quot;Required&quot;">
       <formula>NOT(ISERROR(SEARCH("""Required""",F19)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="37" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="38" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="29" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="30" operator="equal">
       <formula>"No: 300MiB/s is Maximum Supported Load"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="36" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="35" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="27" operator="equal">
       <formula>"""No: 102,400GiB is Maximum Supported Capacity"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="34" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="25" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="26" operator="equal">
       <formula>"No: 102,400GiB is Maximum Supported Capacity"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37 E40">
-    <cfRule type="cellIs" dxfId="32" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="21" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
       <formula>"No: 100,000 IOPS is Maximum Supported Load"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37:G38 F40:G40">
-    <cfRule type="containsText" dxfId="30" priority="18" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="75" priority="18" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",F37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="74" priority="20" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37 E40">
-    <cfRule type="cellIs" dxfId="28" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="19" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31 E20:E23">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="17" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="containsText" dxfId="23" priority="8" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="68" priority="8" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="containsText" dxfId="22" priority="7" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="67" priority="7" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="65" priority="5" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="64" priority="4" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",H19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="61" priority="2" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",H19)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6212,74 +5921,74 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B4">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
       <formula>"No: 300MiB/s is Maximum Supported Load"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",B2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
       <formula>"""No: 102,400GiB is Maximum Supported Capacity"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"No: 102,400GiB is Maximum Supported Capacity"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="No: Required ">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="No: Required ">
       <formula>NOT(ISERROR(SEARCH("No: Required ",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C4">
-    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="No:  Required ">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="No:  Required ">
       <formula>NOT(ISERROR(SEARCH("No:  Required ",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="No:">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="No:">
       <formula>NOT(ISERROR(SEARCH("No:",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C6">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B6">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C6">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8018,6 +7727,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100050FBA8A9F0AFB4BB2D0148D6A234C38" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74183e733b66e5e9a3cd5553bd4bd9ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4a052287-e6d5-446a-afc6-58987b850d5f" xmlns:ns4="943a090e-7b96-4eb7-abc0-264fa36c6c5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b903754823e47922d1d3c75b6236d24" ns3:_="" ns4:_="">
     <xsd:import namespace="4a052287-e6d5-446a-afc6-58987b850d5f"/>
@@ -8240,15 +7958,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7769B51B-49EA-4054-A0C2-A13FF67FB754}">
   <ds:schemaRefs>
@@ -8267,6 +7976,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEC18BF-42E1-4B07-B0F9-328B1505E1A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{097D0541-97F4-46BE-8711-51CFA8DE5931}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8283,12 +8000,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEC18BF-42E1-4B07-B0F9-328B1505E1A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Workbook specifying singleton not supported
Modified workbook specifying single volume or single storage account not supported rather than a general statement of volume or af/apf not supported
</commit_message>
<xml_diff>
--- a/fslogix-storage-calculator.xlsx
+++ b/fslogix-storage-calculator.xlsx
@@ -2,13 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netapp-my.sharepoint.com/personal/mchad_netapp_com/Documents/Documents/DataFabric/calculators/fslogix-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{80057BE8-5265-429A-8C17-C870DB06A720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EEBFEAFB-EFFE-4838-B7E1-BCA353958299}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{02A8BA94-2CA7-429F-88D6-120A4DE887D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3F8B5D34-C872-44B9-BF42-2F439AA1730D}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="ndZNCZJBhvHEZ6ecM4LG4JK89DH8DsJD2GusS6CiAVRt9OjSV2xPKN5fXuzr29rOTpwmNZYdzqFGJkIiNBLh5w==" workbookSaltValue="wC7jlL0OHhGQ9f2ZcebBZw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{CB3913B2-BB8F-4CB3-9459-2FD527F7F31B}"/>
   </bookViews>
@@ -16,8 +17,8 @@
     <sheet name="FSLogix Calculator" sheetId="1" r:id="rId1"/>
     <sheet name="Azure NetApp Files Calcuations" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="Azure Files Calculations" sheetId="4" state="hidden" r:id="rId3"/>
-    <sheet name="definitions" sheetId="2" r:id="rId4"/>
-    <sheet name="Throughput Test" sheetId="5" r:id="rId5"/>
+    <sheet name="definitions" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="Throughput Test" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateCount="3"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="170">
   <si>
     <t>seconds in an hour</t>
   </si>
@@ -246,9 +247,6 @@
     <t>Cost Compared To Azure Premium Files</t>
   </si>
   <si>
-    <t>Supports User Count?</t>
-  </si>
-  <si>
     <t>Monthly Cost Break Down (I/O)</t>
   </si>
   <si>
@@ -477,9 +475,6 @@
     <t>Maximum Tested Bandwidth (MiB/s) At Read %</t>
   </si>
   <si>
-    <t>Required capacity exceeds documented 100TiB upper limit</t>
-  </si>
-  <si>
     <t>Does Calculated Capacity Fit Within Maximum Volume Size? (English)</t>
   </si>
   <si>
@@ -544,6 +539,15 @@
   </si>
   <si>
     <t>Modify: IOPS Per User</t>
+  </si>
+  <si>
+    <t>Required capacity exceeds documented single ANF volume 100TiB upper limit</t>
+  </si>
+  <si>
+    <t>Does Single Storage Account Support User Count?</t>
+  </si>
+  <si>
+    <t>Does Single ANF Volume Support User Count?</t>
   </si>
 </sst>
 </file>
@@ -928,7 +932,355 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="100">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1430,334 +1782,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3610,84 +3634,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{856F6794-4173-4194-B8E4-7BB540367D16}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" tableBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{856F6794-4173-4194-B8E4-7BB540367D16}" name="Table3" displayName="Table3" ref="A2:B9" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98" tableBorderDxfId="97">
   <autoFilter ref="A2:B9" xr:uid="{91E6A135-C0E7-4D0B-8EB4-141892DA45C5}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2F564818-5A0F-4075-8D5E-BCEC57D8FC3C}" name="Fields" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{D42113E7-14D7-4A36-BB89-433CD657FB9D}" name="Input " dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{2F564818-5A0F-4075-8D5E-BCEC57D8FC3C}" name="Fields" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{D42113E7-14D7-4A36-BB89-433CD657FB9D}" name="Input " dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5554924-003B-4661-B33F-97EE2DB8E4A1}" name="Table8" displayName="Table8" ref="A22:B47" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5554924-003B-4661-B33F-97EE2DB8E4A1}" name="Table8" displayName="Table8" ref="A22:B47" totalsRowShown="0" dataDxfId="41">
   <autoFilter ref="A22:B47" xr:uid="{783E58C8-C7D9-4121-86C6-A6F7E49A97E3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{62872274-DD35-4869-BA93-32B33621B006}" name="Keys" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{BCBEE816-C2FF-4BB7-8812-71E8D95CE734}" name="Values" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{62872274-DD35-4869-BA93-32B33621B006}" name="Keys" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{BCBEE816-C2FF-4BB7-8812-71E8D95CE734}" name="Values" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E152E804-6E16-4FE5-822A-359F4049D3B1}" name="Table2" displayName="Table2" ref="A28:B32" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54" tableBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E152E804-6E16-4FE5-822A-359F4049D3B1}" name="Table2" displayName="Table2" ref="A28:B32" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" tableBorderDxfId="92">
   <autoFilter ref="A28:B32" xr:uid="{4897B486-AB3B-4450-B296-0E35971B3AE2}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3A7044B6-6E00-4BEF-9FE6-A7DEE00EE3F3}" name="Azure Files Price Break Down" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{6BB28A88-2884-4CC5-80B3-4CA3051CCAC3}" name="Calculated Output" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{3A7044B6-6E00-4BEF-9FE6-A7DEE00EE3F3}" name="Azure Files Price Break Down" dataDxfId="91"/>
+    <tableColumn id="2" xr3:uid="{6BB28A88-2884-4CC5-80B3-4CA3051CCAC3}" name="Calculated Output" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BA317605-A8C7-4DFA-9894-A955BD37C1CF}" name="Table4" displayName="Table4" ref="A11:B16" totalsRowShown="0" headerRowDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BA317605-A8C7-4DFA-9894-A955BD37C1CF}" name="Table4" displayName="Table4" ref="A11:B16" totalsRowShown="0" headerRowDxfId="89" tableBorderDxfId="88">
   <autoFilter ref="A11:B16" xr:uid="{FDD62D26-CF49-4DB8-BB86-E5640AFB3072}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{98F6AE4C-A8FE-46A2-B695-4F7EC29B79C1}" name="High Level Environmental Needs" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{923448D6-8587-46CF-AC83-4786C0E6E31A}" name="Calculated Output" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{98F6AE4C-A8FE-46A2-B695-4F7EC29B79C1}" name="High Level Environmental Needs" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{923448D6-8587-46CF-AC83-4786C0E6E31A}" name="Calculated Output" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E9B81EED-ACF0-4F74-94BF-2331D9B58AEF}" name="Table5" displayName="Table5" ref="A36:B38" totalsRowShown="0" dataDxfId="46" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E9B81EED-ACF0-4F74-94BF-2331D9B58AEF}" name="Table5" displayName="Table5" ref="A36:B38" totalsRowShown="0" dataDxfId="85" tableBorderDxfId="84">
   <autoFilter ref="A36:B38" xr:uid="{F64951B7-0541-475C-8E4E-15CB609631E0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{EEA382B5-FB82-4F1D-9327-A87385C52897}" name="Azure Premium Files Price Break Down" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{E770553C-A0C0-45E6-BC23-3E0DD3249B14}" name="Calculated Output" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{EEA382B5-FB82-4F1D-9327-A87385C52897}" name="Azure Premium Files Price Break Down" dataDxfId="83"/>
+    <tableColumn id="2" xr3:uid="{E770553C-A0C0-45E6-BC23-3E0DD3249B14}" name="Calculated Output" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{72039F74-6304-436F-9B2C-E726744D9970}" name="Table9" displayName="Table9" ref="A18:B22" totalsRowShown="0" dataDxfId="42" tableBorderDxfId="41">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{72039F74-6304-436F-9B2C-E726744D9970}" name="Table9" displayName="Table9" ref="A18:B22" totalsRowShown="0" dataDxfId="81" tableBorderDxfId="80">
   <autoFilter ref="A18:B22" xr:uid="{1849FF8B-C5DF-48B3-BD49-7E1B6D720287}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3F78E685-9C28-44F6-9A2A-3F9135F54C28}" name="Azure NetApp Files Price Break Down" dataDxfId="40"/>
-    <tableColumn id="2" xr3:uid="{AA370671-CA18-4101-A4C3-7BC422CCC1F1}" name="Calculated Output" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{3F78E685-9C28-44F6-9A2A-3F9135F54C28}" name="Azure NetApp Files Price Break Down" dataDxfId="79"/>
+    <tableColumn id="2" xr3:uid="{AA370671-CA18-4101-A4C3-7BC422CCC1F1}" name="Calculated Output" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{2F4EE936-97FF-430B-BCE0-3BA4433FF3D4}" name="Table91119" displayName="Table91119" ref="D18:H26" totalsRowShown="0" dataDxfId="38" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{2F4EE936-97FF-430B-BCE0-3BA4433FF3D4}" name="Table91119" displayName="Table91119" ref="D18:H26" totalsRowShown="0" dataDxfId="77" tableBorderDxfId="76">
   <autoFilter ref="D18:H26" xr:uid="{F75E429C-8018-41C4-B4C3-C0AD783F2D38}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{25D43E32-76CE-4E57-9637-4A7FD2463E37}" name="Azure NetApp Files Additional Information" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{3C9CF5B6-EAB8-4222-9C96-5A10EE28F85F}" name=" Output" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{F8FAE1CB-5733-4CC5-9F68-AD29EB511AF6}" name="Etc(1)" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{25D43E32-76CE-4E57-9637-4A7FD2463E37}" name="Azure NetApp Files Additional Information" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{3C9CF5B6-EAB8-4222-9C96-5A10EE28F85F}" name=" Output" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{F8FAE1CB-5733-4CC5-9F68-AD29EB511AF6}" name="Etc(1)" dataDxfId="72">
       <calculatedColumnFormula>IF(E20&gt;definitions!B24,definitions!$A$23,"Yes")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2A8935D0-2756-4A0D-B01F-87C8DFAE1AD5}" name="Etc(2)" dataDxfId="32">
+    <tableColumn id="4" xr3:uid="{2A8935D0-2756-4A0D-B01F-87C8DFAE1AD5}" name="Etc(2)" dataDxfId="71">
       <calculatedColumnFormula>IF(B3&gt;E24,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7CD54AC1-822B-4FE1-B7D3-C9A779DEF8FC}" name="Etc(3)" dataDxfId="31">
+    <tableColumn id="5" xr3:uid="{7CD54AC1-822B-4FE1-B7D3-C9A779DEF8FC}" name="Etc(3)" dataDxfId="70">
       <calculatedColumnFormula>IF(B3&gt;E24,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3696,18 +3720,18 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{E617B910-6016-4284-B1B7-B2BDBB2DAC94}" name="Table622" displayName="Table622" ref="D28:H34" totalsRowShown="0" headerRowDxfId="30" tableBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{E617B910-6016-4284-B1B7-B2BDBB2DAC94}" name="Table622" displayName="Table622" ref="D28:H34" totalsRowShown="0" headerRowDxfId="69" tableBorderDxfId="68">
   <autoFilter ref="D28:H34" xr:uid="{6432D5DC-E020-4F4A-81F0-AFAE2FFBB2FE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{284AB7F5-C1F5-4923-8D18-8B326F2B7795}" name="Azure Standard Files Additional Information"/>
-    <tableColumn id="2" xr3:uid="{A95529E7-EF42-4D6F-BDD9-4D129864E797}" name="Output" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{9881ABB1-4E08-4030-AEC9-CCA810605C29}" name="Etc(1)" dataDxfId="27">
+    <tableColumn id="2" xr3:uid="{A95529E7-EF42-4D6F-BDD9-4D129864E797}" name="Output" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{9881ABB1-4E08-4030-AEC9-CCA810605C29}" name="Etc(1)" dataDxfId="66">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5BC3DEF6-CDB9-4DE9-B8FF-9749CBA220CD}" name="Etc(2)" dataDxfId="26">
+    <tableColumn id="4" xr3:uid="{5BC3DEF6-CDB9-4DE9-B8FF-9749CBA220CD}" name="Etc(2)" dataDxfId="65">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3F802064-6239-4D79-9EEF-E6B1422584F4}" name="Etc(3)" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{3F802064-6239-4D79-9EEF-E6B1422584F4}" name="Etc(3)" dataDxfId="64">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3716,15 +3740,15 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{017E12BE-FEED-449C-A993-3E3DA447FC83}" name="Table61423" displayName="Table61423" ref="D36:G42" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{017E12BE-FEED-449C-A993-3E3DA447FC83}" name="Table61423" displayName="Table61423" ref="D36:G42" totalsRowShown="0" headerRowDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="D36:G42" xr:uid="{35197520-871D-45A1-92D2-3E64562C597C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7454E181-1F78-43D7-992D-393BF7E62908}" name="Azure Premium Files Additional Information"/>
-    <tableColumn id="2" xr3:uid="{D283543A-6DF3-46B8-B880-680345E5383E}" name="output" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{383E5A06-7313-4E3D-A474-C65E865DB16D}" name="Etc(1)" dataDxfId="21">
+    <tableColumn id="2" xr3:uid="{D283543A-6DF3-46B8-B880-680345E5383E}" name="output" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{383E5A06-7313-4E3D-A474-C65E865DB16D}" name="Etc(1)" dataDxfId="60">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{22B7B0DB-CD46-43E2-A4B8-192176C63B53}" name="Etc(2)" dataDxfId="20">
+    <tableColumn id="4" xr3:uid="{22B7B0DB-CD46-43E2-A4B8-192176C63B53}" name="Etc(2)" dataDxfId="59">
       <calculatedColumnFormula>'Azure Files Calculations'!$B$5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3739,7 +3763,7 @@
     <tableColumn id="2" xr3:uid="{9191646A-D382-43C8-AD5D-D9379A6352B8}" name="IO Size"/>
     <tableColumn id="3" xr3:uid="{B94E1025-3714-4DA4-824F-A38F565F77F4}" name="IOPS Per User"/>
     <tableColumn id="1" xr3:uid="{E67A9471-95D1-42FF-B18E-7D012DE67FD4}" name="VHD Sizes"/>
-    <tableColumn id="4" xr3:uid="{779397D8-86EA-41AE-9217-A6D49A13139B}" name="Concurrent Users" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{779397D8-86EA-41AE-9217-A6D49A13139B}" name="Concurrent Users" dataDxfId="42"/>
     <tableColumn id="5" xr3:uid="{5EBEBC80-5940-4420-B7CB-91D5FC7DF075}" name="Read Percenage"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4043,19 +4067,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594F1148-3B87-4101-8535-9F7FDD18F1E9}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" customWidth="1"/>
     <col min="4" max="4" width="85.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
@@ -4066,7 +4090,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="78"/>
     </row>
@@ -4083,12 +4107,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="32">
-        <v>118</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B4" s="32">
         <v>15</v>
@@ -4100,12 +4124,12 @@
         <v>63</v>
       </c>
       <c r="B5" s="32">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="47">
         <v>1</v>
@@ -4123,7 +4147,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B8" s="32">
         <v>32</v>
@@ -4133,7 +4157,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9" s="62">
         <v>0.2</v>
@@ -4157,16 +4181,16 @@
       </c>
       <c r="B12" s="18">
         <f>B$3*B$6</f>
-        <v>118</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="18">
         <f>(B$4*B$8*B$3*B$6)/1024</f>
-        <v>55.3125</v>
+        <v>64.21875</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -4184,7 +4208,7 @@
       </c>
       <c r="B15" s="18">
         <f>B$4*B$3*B6</f>
-        <v>1770</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -4193,12 +4217,12 @@
       </c>
       <c r="B16" s="18">
         <f>B5*B3</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="79" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="79"/>
       <c r="C17" s="79"/>
@@ -4210,16 +4234,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
         <v>57</v>
@@ -4231,16 +4255,16 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="51" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="51" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="54">
-        <f>IF(E19="Yes",_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!C$38:C$40,'Azure NetApp Files Calcuations'!B$38:B$40,definitions!A$23),"N/A: User Count Excceds Capability Of Azure NetApp Files")</f>
-        <v>619.5</v>
+        <f>IF(E19="Yes",_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!C$38:C$40,'Azure NetApp Files Calcuations'!B$38:B$40,definitions!A$23),"N/A: User Count Excceds Capability Of Single Azure NetApp Files Volume")</f>
+        <v>616.5</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>69</v>
+        <v>169</v>
       </c>
       <c r="E19" s="48" t="str">
         <f>_xlfn.XLOOKUP("No",'Azure NetApp Files Calcuations'!B35:B36,'Azure NetApp Files Calcuations'!B35:B36,"Yes")</f>
@@ -4252,24 +4276,24 @@
       </c>
       <c r="G19" s="66"/>
       <c r="H19" s="65" t="str">
-        <f>IF(B3&gt;E24,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</f>
+        <f>IF(B3&gt;E24,"Required bandwidth exceeds single ANF volume tested upper limit at selected read percentage","Yes")</f>
         <v>Yes</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B20" s="49">
         <f>IF(E19="Yes",IF($E$21=definitions!A$23,B$19,B$19/B$3),"N/A: User Count Excceds Capability Of Azure NetApp Files")</f>
-        <v>5.25</v>
+        <v>4.5</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E20" s="52">
         <f>IF('Azure NetApp Files Calcuations'!B35="Yes",_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!$C$31:$C$33,'Azure NetApp Files Calcuations'!$B$31:$B$33),"No")</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="F20" s="53"/>
       <c r="G20" s="67"/>
@@ -4281,10 +4305,10 @@
       </c>
       <c r="B21" s="50">
         <f>IF(E29="Yes",_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!C$46:C$48,'Azure NetApp Files Calcuations'!B$46:B$48),"N/A: User Count Exceeds Capability Of Azure Files")</f>
-        <v>1.4982876712328768</v>
+        <v>1.404494382022472</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E21" s="52" t="str">
         <f>IF('Azure NetApp Files Calcuations'!B35="Yes",(_xlfn.XLOOKUP(MIN('Azure NetApp Files Calcuations'!$B$38:$B$40),'Azure NetApp Files Calcuations'!$B$38:$B$40,'Azure NetApp Files Calcuations'!$C$38:$C$40)),"No")</f>
@@ -4303,11 +4327,11 @@
         <v>0.6</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E22" s="52" t="str">
         <f>IF(E19="No","No",(_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!$C$27:$C$29,'Azure NetApp Files Calcuations'!$B$27:$B$29)))</f>
-        <v>Capacity</v>
+        <v>Bandwidth</v>
       </c>
       <c r="F22" s="53"/>
       <c r="G22" s="67"/>
@@ -4317,11 +4341,11 @@
       <c r="A23" s="35"/>
       <c r="B23" s="50"/>
       <c r="D23" s="35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E23" s="52">
         <f>IF(E19="Yes",(_xlfn.XLOOKUP(E21,'Azure NetApp Files Calcuations'!$C$42:$C$44,'Azure NetApp Files Calcuations'!$B$42:$B$44,definitions!A$23)),"No")</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F23" s="53"/>
       <c r="G23" s="67"/>
@@ -4331,7 +4355,7 @@
       <c r="A24" s="35"/>
       <c r="B24" s="49"/>
       <c r="D24" s="64" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24" s="69">
         <f>FLOOR(('Azure NetApp Files Calcuations'!B4*1024/'FSLogix Calculator'!B14)*(1/'FSLogix Calculator'!B6),1)</f>
@@ -4345,15 +4369,15 @@
       <c r="A25" s="35"/>
       <c r="B25" s="49"/>
       <c r="D25" s="64" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E25" s="69">
         <f>'Azure NetApp Files Calcuations'!B5</f>
-        <v>2925</v>
+        <v>3413</v>
       </c>
       <c r="F25" s="68" t="str">
         <f>IF(E26&gt;definitions!B30,definitions!$A$23,"Yes")</f>
-        <v>Required capacity exceeds documented 100TiB upper limit</v>
+        <v>Required capacity exceeds documented single ANF volume 100TiB upper limit</v>
       </c>
       <c r="G25" s="68" t="str">
         <f>IF(B9&gt;E28,"Required bandwidth exceeds tested upper limit at selected read percentage","Yes")</f>
@@ -4381,7 +4405,7 @@
     </row>
     <row r="27" spans="1:8" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" s="79"/>
       <c r="C27" s="79"/>
@@ -4393,16 +4417,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F28" s="58" t="s">
         <v>57</v>
@@ -4414,16 +4438,16 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B29" s="54">
-        <f>IF(E29="Yes",B$32+B$31,"N/A: User Count Exceeds Capability Of Azure Files")</f>
-        <v>413.47199999999998</v>
+        <f>IF(E29="Yes",B$32+B$31,"N/A: User Count Exceeds Capability Of Single Azure Files Storage Account")</f>
+        <v>438.94799999999998</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>69</v>
+        <v>168</v>
       </c>
       <c r="E29" s="35" t="str">
         <f>_xlfn.XLOOKUP("No",'Azure Files Calculations'!$C$2:$C$4,'Azure Files Calculations'!$C$2:$C$4,"Yes")</f>
@@ -4444,18 +4468,18 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="49">
         <f>IF(E29="Yes",B$29/B$3,"N/A: User Count Exceeds Capability Of Azure Files")</f>
-        <v>3.504</v>
+        <v>3.2039999999999997</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="18">
         <f>IF(E29="Yes",$B$5*$B$3,"No")</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="F30" s="40"/>
       <c r="G30" s="39"/>
@@ -4463,18 +4487,18 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="49">
         <f>IF(E29="Yes",((B4*B3*B6*definitions!B$32*B$7*definitions!B$34)/definitions!B33)*definitions!B$36,"N/A: User Count Exceeds Capability Of Azure Files")</f>
-        <v>165.672</v>
+        <v>192.34799999999998</v>
       </c>
       <c r="D31" s="27" t="s">
         <v>66</v>
       </c>
       <c r="E31" s="18">
         <f>IF(E29="Yes",E30/$B$3,"No")</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F31" s="40"/>
       <c r="G31" s="43"/>
@@ -4482,14 +4506,14 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="49">
         <f>IF(E29="Yes",B$5*B$3*B6*definitions!B$35,"N/A: User Count Exceeds Capability Of Azure Files")</f>
-        <v>247.79999999999998</v>
+        <v>246.6</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E32" s="18">
         <f>FLOOR(   (definitions!$B$38/$B$4)*(1/$B$6),1)</f>
@@ -4503,7 +4527,7 @@
       <c r="A33" s="35"/>
       <c r="B33" s="49"/>
       <c r="D33" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E33" s="18">
         <f>FLOOR((   (1024*definitions!$B$39)   /   ('FSLogix Calculator'!$B$4*'FSLogix Calculator'!$B$8)  ) * (1/$B$6   ),1)</f>
@@ -4515,11 +4539,11 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D34" s="64" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E34" s="17">
         <f>definitions!B41/'FSLogix Calculator'!B5</f>
-        <v>2925.7142857142858</v>
+        <v>3413.3333333333335</v>
       </c>
       <c r="F34" s="70"/>
       <c r="G34" s="70"/>
@@ -4527,7 +4551,7 @@
     </row>
     <row r="35" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="79" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" s="79"/>
       <c r="C35" s="79"/>
@@ -4538,16 +4562,16 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F36" t="s">
         <v>57</v>
@@ -4556,16 +4580,16 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B37" s="54">
-        <f>IF(E37="Yes",IF(E40="I/O Need",definitions!B37*'FSLogix Calculator'!B3*'FSLogix Calculator'!B4,definitions!B37*'FSLogix Calculator'!B5*'FSLogix Calculator'!B3),"N/A: User Count Exceeds Capability Of Azure Premium Files")</f>
-        <v>1032.5</v>
+        <f>IF(E37="Yes",IF(E40="I/O Need",definitions!B37*'FSLogix Calculator'!B3*'FSLogix Calculator'!B4,definitions!B37*'FSLogix Calculator'!B5*'FSLogix Calculator'!B3),"N/A: User Count Exceeds Capability Of Single Azure Premium Files Storage Account")</f>
+        <v>1027.5</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>69</v>
+        <v>168</v>
       </c>
       <c r="E37" s="35" t="str">
         <f>_xlfn.XLOOKUP("No",'Azure Files Calculations'!$C$5:$C$7,'Azure Files Calculations'!$C$2:$C$4,"Yes")</f>
@@ -4582,29 +4606,29 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" s="23">
         <f>IF(E37="Yes",B$37/B$3,"N/A: User Count Exceeds Capability Of Azure Premium Files")</f>
-        <v>8.75</v>
+        <v>7.5</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E38" s="18">
         <f>'Azure Files Calculations'!C14</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="F38" s="42"/>
       <c r="G38" s="42"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D39" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E39" s="17">
         <f>IF('Azure Files Calculations'!$C$6="Yes",E$38/$B$3,"No")</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F39" s="33"/>
       <c r="G39" s="41"/>
@@ -4614,7 +4638,7 @@
       <c r="B40" s="17"/>
       <c r="C40" s="8"/>
       <c r="D40" s="27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E40" s="22" t="str">
         <f>'Azure Files Calculations'!B14</f>
@@ -4628,7 +4652,7 @@
       <c r="B41" s="17"/>
       <c r="C41" s="8"/>
       <c r="D41" s="27" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E41" s="18">
         <f>FLOOR(( definitions!$B$40/$B$4) * (1/$B$6),1)</f>
@@ -4640,11 +4664,11 @@
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="8"/>
       <c r="D42" s="64" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E42" s="18">
         <f>definitions!B42/'FSLogix Calculator'!B5</f>
-        <v>2925.7142857142858</v>
+        <v>3413.3333333333335</v>
       </c>
       <c r="F42" s="40"/>
       <c r="G42" s="45"/>
@@ -4893,7 +4917,7 @@
       <c r="E112" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vjT6CCKfIrO/jXzdur1RhpGnjRqhL+DaQXy52zAi/TSyztQjEWBS2QXCVfbW28nJMhsff53LBSETI75V5qR4rw==" saltValue="dqYSPUVkn4pwwVpSznIOyA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Utg0jyYNPar1KiVw45ZuSBHkoWRsVvJh5UJ/K82/yMS7SVS5OBRS9+rF29DL8t2cU+gBNU7SEFaKXJSfD/VFBg==" saltValue="C+TzLKWEZ0rE1g4FfHefcw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A27:H27"/>
@@ -4902,163 +4926,169 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A36:B39 A28:B34">
-    <cfRule type="cellIs" dxfId="97" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="95" operator="equal">
       <formula>"Temporarily Empty Field"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:H31">
-    <cfRule type="containsText" dxfId="96" priority="23" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="37" priority="25" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="24" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="36" priority="26" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",F29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E23">
-    <cfRule type="cellIs" dxfId="94" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
       <formula>"Capacity Pool Minimum Size"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="93" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
       <formula>"Temporarily Empty Field"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="92" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="41" operator="equal">
       <formula>"Temporarily Empty Field"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="91" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="34" operator="equal">
       <formula>"""Yes"""</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="88" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>"Required Capacity Exceeds documented 100TiB Upper Limit"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
       <formula>"""Required Capacity Exceeds documented 100TiB Upper Limit"""</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="35" operator="containsText" text="&quot;Required&quot;">
+    <cfRule type="containsText" dxfId="27" priority="37" operator="containsText" text="&quot;Required&quot;">
       <formula>NOT(ISERROR(SEARCH("""Required""",F19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="36" operator="containsText" text="&quot;Required&quot;">
+    <cfRule type="containsText" dxfId="26" priority="38" operator="containsText" text="&quot;Required&quot;">
       <formula>NOT(ISERROR(SEARCH("""Required""",F19)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="39" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="Required">
+      <formula>NOT(ISERROR(SEARCH("Required",F19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
+      <formula>"No: 300MiB/s is Maximum Supported Load"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="83" priority="29" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="30" operator="equal">
-      <formula>"No: 300MiB/s is Maximum Supported Load"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="81" priority="28" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="80" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="29" operator="equal">
       <formula>"""No: 102,400GiB is Maximum Supported Capacity"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="cellIs" dxfId="79" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
       <formula>"No: 102,400GiB is Maximum Supported Capacity"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37 E40">
-    <cfRule type="cellIs" dxfId="77" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
       <formula>"No: 100,000 IOPS is Maximum Supported Load"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37:G38 F40:G40">
-    <cfRule type="containsText" dxfId="75" priority="18" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",F37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="20" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37 E40">
-    <cfRule type="cellIs" dxfId="73" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31 E20:E23">
-    <cfRule type="cellIs" dxfId="72" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="cellIs" dxfId="71" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="cellIs" dxfId="70" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="cellIs" dxfId="69" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="containsText" dxfId="68" priority="8" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="containsText" dxfId="67" priority="7" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="65" priority="5" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="64" priority="4" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",B30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",H19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="2" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Required">
+      <formula>NOT(ISERROR(SEARCH("Required",H19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",H19)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5166,6 +5196,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E156B8-3DAB-4F24-8D0A-36FBCF57BCBD}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
@@ -5190,23 +5221,23 @@
       </c>
       <c r="B2" s="15">
         <f>'FSLogix Calculator'!B$16</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="15">
         <f>'FSLogix Calculator'!B$5</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B4" s="2">
         <f>_xlfn.XLOOKUP('FSLogix Calculator'!B$9,'Throughput Test'!G2:G12,'Throughput Test'!P$2:P$12)</f>
@@ -5216,11 +5247,11 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B5" s="2">
         <f>FLOOR(definitions!B24/'FSLogix Calculator'!B$5,1)</f>
-        <v>2925</v>
+        <v>3413</v>
       </c>
       <c r="C5" s="61"/>
     </row>
@@ -5235,7 +5266,7 @@
       </c>
       <c r="B7" s="15">
         <f>('FSLogix Calculator'!B$13*1024)/definitions!B30</f>
-        <v>3540</v>
+        <v>4110</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>46</v>
@@ -5247,7 +5278,7 @@
       </c>
       <c r="B8" s="15">
         <f>('FSLogix Calculator'!B$13*1024)/definitions!B28</f>
-        <v>885</v>
+        <v>1027.5</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>47</v>
@@ -5259,7 +5290,7 @@
       </c>
       <c r="B9" s="15">
         <f>('FSLogix Calculator'!B$13*1024)/definitions!B26</f>
-        <v>442.5</v>
+        <v>513.75</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>39</v>
@@ -5267,7 +5298,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B11" s="2">
         <f>('FSLogix Calculator'!B$14*'FSLogix Calculator'!B$6)/definitions!B$30</f>
@@ -5279,7 +5310,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="2">
         <f>('FSLogix Calculator'!B$14*'FSLogix Calculator'!B$6)/definitions!B28</f>
@@ -5291,7 +5322,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="2">
         <f>('FSLogix Calculator'!B$14*'FSLogix Calculator'!B$6)/definitions!B26</f>
@@ -5312,7 +5343,7 @@
       </c>
       <c r="B15" s="2">
         <f>CEILING(IF(B11&gt;B$3,definitions!B$31/B11,definitions!B$31/B$3),1)</f>
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>46</v>
@@ -5324,7 +5355,7 @@
       </c>
       <c r="B16" s="2">
         <f>CEILING(IF(B12&gt;B$3,definitions!B$31/B12,definitions!B$31/B$3),1)</f>
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>47</v>
@@ -5336,7 +5367,7 @@
       </c>
       <c r="B17" s="2">
         <f>CEILING(IF(B13&gt;B$3,definitions!B$31/B13,definitions!B$31/B$3),1)</f>
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>39</v>
@@ -5349,11 +5380,11 @@
     </row>
     <row r="19" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="15" t="str">
         <f>IF(B$2&gt;B7,"Capacity","Bandwidth")</f>
-        <v>Capacity</v>
+        <v>Bandwidth</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>46</v>
@@ -5361,7 +5392,7 @@
     </row>
     <row r="20" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="15" t="str">
         <f>IF(B$2&gt;B8,"Capacity","Bandwidth")</f>
@@ -5373,7 +5404,7 @@
     </row>
     <row r="21" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="15" t="str">
         <f>IF(B$2&gt;B9,"Capacity","Bandwidth")</f>
@@ -5390,11 +5421,11 @@
     </row>
     <row r="23" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="15">
         <f>IF(B$2&gt;B7,B$2,B7)</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>46</v>
@@ -5402,11 +5433,11 @@
     </row>
     <row r="24" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" s="15">
         <f>IF(B$2&gt;B8,B$2,B8)</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>47</v>
@@ -5414,11 +5445,11 @@
     </row>
     <row r="25" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25" s="15">
         <f>IF(B$2&gt;B9,B$2,B9)</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>39</v>
@@ -5431,11 +5462,11 @@
     </row>
     <row r="27" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" s="15" t="str">
         <f>IF(B23&gt;definitions!B$31,B19,"Capacity Pool Minimum Size")</f>
-        <v>Capacity</v>
+        <v>Bandwidth</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>46</v>
@@ -5443,7 +5474,7 @@
     </row>
     <row r="28" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="15" t="str">
         <f>IF(B24&gt;definitions!B$31,B20,"Capacity Pool Minimum Size")</f>
@@ -5455,7 +5486,7 @@
     </row>
     <row r="29" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" s="15" t="str">
         <f>IF(B25&gt;definitions!B$31,B21,"Capacity Pool Minimum Size")</f>
@@ -5472,11 +5503,11 @@
     </row>
     <row r="31" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31" s="15">
         <f>IF(B23&gt;definitions!B$31,B23,definitions!B$31)</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>46</v>
@@ -5484,11 +5515,11 @@
     </row>
     <row r="32" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="15">
         <f>IF(B24&gt;definitions!B$31,B24,definitions!B$31)</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>47</v>
@@ -5496,11 +5527,11 @@
     </row>
     <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33" s="15">
         <f>IF(B25&gt;definitions!B$31,B25,definitions!B$31)</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>39</v>
@@ -5513,7 +5544,7 @@
     </row>
     <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B35" s="15" t="str">
         <f>IF(MIN(B31:B33)&gt;definitions!B24,"No","Yes")</f>
@@ -5523,7 +5554,7 @@
     </row>
     <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B36" s="2" t="str">
         <f>IF('FSLogix Calculator'!B3&gt;('FSLogix Calculator'!E24),"No","Yes")</f>
@@ -5546,7 +5577,7 @@
       </c>
       <c r="B38" s="24">
         <f>IF((B31&gt;definitions!B24),99999,B31*definitions!B$29)</f>
-        <v>619.5</v>
+        <v>616.5</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>46</v>
@@ -5560,7 +5591,7 @@
       </c>
       <c r="B39" s="16">
         <f>IF((B32&gt;definitions!B24),99999,B32*definitions!B$27)</f>
-        <v>1239</v>
+        <v>1233</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>47</v>
@@ -5574,7 +5605,7 @@
       </c>
       <c r="B40" s="16">
         <f>IF((B33&gt;definitions!B24),99999,(B33*definitions!B$25))</f>
-        <v>1652</v>
+        <v>1644</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>39</v>
@@ -5595,7 +5626,7 @@
       </c>
       <c r="B42" s="15">
         <f>B31/'FSLogix Calculator'!B$3</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>46</v>
@@ -5609,7 +5640,7 @@
       </c>
       <c r="B43" s="15">
         <f>B32/'FSLogix Calculator'!B$3</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>47</v>
@@ -5623,7 +5654,7 @@
       </c>
       <c r="B44" s="15">
         <f>B33/'FSLogix Calculator'!B$3</f>
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>39</v>
@@ -5644,7 +5675,7 @@
       </c>
       <c r="B46" s="26">
         <f>IF(B38=definitions!A$23,B38, B38/'FSLogix Calculator'!B$29)</f>
-        <v>1.4982876712328768</v>
+        <v>1.404494382022472</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>46</v>
@@ -5658,7 +5689,7 @@
       </c>
       <c r="B47" s="26">
         <f>IF(B39=definitions!A$23,B39, B39/'FSLogix Calculator'!B$29)</f>
-        <v>2.9965753424657535</v>
+        <v>2.808988764044944</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>47</v>
@@ -5672,7 +5703,7 @@
       </c>
       <c r="B48" s="26">
         <f>IF(B40=definitions!A$23,B40, B40/'FSLogix Calculator'!B$29)</f>
-        <v>3.9954337899543382</v>
+        <v>3.7453183520599254</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>39</v>
@@ -5727,7 +5758,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="76" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B54">
         <f>FLOOR(('Azure NetApp Files Calcuations'!B4*1024/'FSLogix Calculator'!B14)*(1/'FSLogix Calculator'!B6),1)</f>
@@ -5741,10 +5772,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E85F820-7E22-48AB-88D3-5118FCDA0E46}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5767,7 +5799,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="36" t="str">
-        <f>IF('FSLogix Calculator'!B15&gt;definitions!B$38,"Required I/O rate exceeds documented 10,000 op rate upper limit","Yes")</f>
+        <f>IF('FSLogix Calculator'!B15&gt;definitions!B$38,"Required I/O rate exceeds documented single storage account 10,000 op rate upper limit","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C2" s="37" t="str">
@@ -5780,7 +5812,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="38" t="str">
-        <f>IF(('FSLogix Calculator'!B13)&gt;definitions!B$39,"Required bandwidth exceeds documented 300MiB/s  upper limit","Yes")</f>
+        <f>IF(('FSLogix Calculator'!B13)&gt;definitions!B$39,"Required bandwidth exceeds documented single storage account 300MiB/s  upper limit","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C3" s="37" t="str">
@@ -5793,7 +5825,7 @@
         <v>38</v>
       </c>
       <c r="B4" s="36" t="str">
-        <f>IF('FSLogix Calculator'!B16&gt;102400,"Required capacity exceeds documented 100TiB upper limit","Yes")</f>
+        <f>IF('FSLogix Calculator'!B16&gt;102400,"Required capacity exceeds documented single storage account 100TiB upper limit","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C4" s="37" t="str">
@@ -5806,7 +5838,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="37" t="str">
-        <f>IF(('FSLogix Calculator'!B$4*'FSLogix Calculator'!B$3*'FSLogix Calculator'!B$6)&gt;definitions!B$40,"Required I/O rate exceeds documented 100,000 op rate upper limit","Yes")</f>
+        <f>IF(('FSLogix Calculator'!B$4*'FSLogix Calculator'!B$3*'FSLogix Calculator'!B$6)&gt;definitions!B$40,"Required I/O rate exceeds documented single storage account 100,000 op rate upper limit","Yes")</f>
         <v>Yes</v>
       </c>
       <c r="C5" s="37" t="str">
@@ -5816,7 +5848,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="37" t="str">
         <f>IF(IF(('FSLogix Calculator'!$B$4*'FSLogix Calculator'!$B$3*'FSLogix Calculator'!$B$6)&gt;('FSLogix Calculator'!$B$5*'FSLogix Calculator'!$B$3),'FSLogix Calculator'!$B$4*'FSLogix Calculator'!$B$3*'FSLogix Calculator'!$B$6,'FSLogix Calculator'!$B$5*'FSLogix Calculator'!$B$3)&gt;definitions!B42,"Required capacity exceeds documented 100TiB upper limit","Yes")</f>
@@ -5834,49 +5866,49 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" s="15">
         <f>(('FSLogix Calculator'!B13-('FSLogix Calculator'!B13*(1-'FSLogix Calculator'!B9)))-definitions!B43)/definitions!B44</f>
-        <v>-815.625</v>
+        <v>-785.9375</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B9" s="15">
         <f>(('FSLogix Calculator'!B13-('FSLogix Calculator'!B13*'FSLogix Calculator'!B9))-definitions!B45)/definitions!B46</f>
-        <v>106.25</v>
+        <v>284.375</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B10" s="15">
         <f>IF(B8&lt;100,100,B8)</f>
         <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B11" s="15">
         <f>IF(B9&lt;100,100,B9)</f>
-        <v>106.25</v>
+        <v>284.375</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B12" t="str">
         <f>_xlfn.XLOOKUP(MAX(B10:B11),B10:B11,C10:C11)</f>
@@ -5884,12 +5916,12 @@
       </c>
       <c r="C12" s="15">
         <f>MAX(B10:B11)</f>
-        <v>106.25</v>
+        <v>284.375</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B13" t="str">
         <f>IF(B9&gt;'FSLogix Calculator'!B3*'FSLogix Calculator'!B4*'FSLogix Calculator'!B6,"Bandwidth Need","I/O Need")</f>
@@ -5897,12 +5929,12 @@
       </c>
       <c r="C13" s="15">
         <f>IF(B9&gt;'FSLogix Calculator'!B3*'FSLogix Calculator'!B4*'FSLogix Calculator'!B6,C$12,'FSLogix Calculator'!B3*'FSLogix Calculator'!B4*'FSLogix Calculator'!B6)</f>
-        <v>1770</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B14" t="str">
         <f>IF(C13&gt;'FSLogix Calculator'!B16,'Azure Files Calculations'!B13,"Profile Size")</f>
@@ -5910,7 +5942,7 @@
       </c>
       <c r="C14" s="15">
         <f>IF(C13&gt;'FSLogix Calculator'!B16,'Azure Files Calculations'!C13,'FSLogix Calculator'!B16)</f>
-        <v>4130</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -5921,74 +5953,74 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B4">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="15" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="16" operator="equal">
       <formula>"No: 300MiB/s is Maximum Supported Load"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="17" priority="14" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="56" priority="14" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="55" priority="4" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="54" priority="5" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",B2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="13" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="12" operator="equal">
       <formula>"""No: 102,400GiB is Maximum Supported Capacity"""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="11" operator="equal">
       <formula>"No: 102,400GiB is Maximum Supported Capacity"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="10" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C4">
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="No: Required ">
+    <cfRule type="containsText" dxfId="48" priority="8" operator="containsText" text="No: Required ">
       <formula>NOT(ISERROR(SEARCH("No: Required ",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C4">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="No:  Required ">
+    <cfRule type="containsText" dxfId="47" priority="7" operator="containsText" text="No:  Required ">
       <formula>NOT(ISERROR(SEARCH("No:  Required ",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="No:">
+    <cfRule type="containsText" dxfId="46" priority="6" operator="containsText" text="No:">
       <formula>NOT(ISERROR(SEARCH("No:",C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C6">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B6">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C6">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Required">
+    <cfRule type="containsText" dxfId="43" priority="1" operator="containsText" text="Required">
       <formula>NOT(ISERROR(SEARCH("Required",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5998,10 +6030,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8274658-AC29-4B53-B5B1-54B6D412C541}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6026,7 +6059,7 @@
         <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6194,7 +6227,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="B23" s="2"/>
       <c r="D23" s="46"/>
@@ -6349,7 +6382,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B41" s="15">
         <v>102400</v>
@@ -6357,7 +6390,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B42" s="15">
         <v>102400</v>
@@ -6365,7 +6398,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B43" s="15">
         <v>60</v>
@@ -6373,7 +6406,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B44" s="73">
         <v>0.06</v>
@@ -6381,7 +6414,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B45" s="15">
         <v>40</v>
@@ -6389,7 +6422,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B46" s="73">
         <v>0.04</v>
@@ -6397,7 +6430,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B47" s="26">
         <v>0.4</v>
@@ -6414,10 +6447,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA9B902-59E6-4153-97E0-22C91333C597}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AI12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G12"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6432,120 +6466,120 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
         <v>127</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>128</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>129</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>131</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>132</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>133</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>134</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>135</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>136</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>137</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>138</v>
       </c>
-      <c r="M1" t="s">
-        <v>139</v>
-      </c>
       <c r="N1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" t="s">
         <v>129</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>130</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>131</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>132</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>133</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>134</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>135</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>136</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>137</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>138</v>
       </c>
-      <c r="X1" t="s">
-        <v>139</v>
-      </c>
       <c r="Y1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z1" t="s">
         <v>129</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>130</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>131</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>132</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>133</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>134</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>135</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>136</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>137</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>138</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
         <v>113</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>114</v>
-      </c>
-      <c r="C2" t="s">
-        <v>115</v>
       </c>
       <c r="D2">
         <v>9027</v>
@@ -6578,7 +6612,7 @@
         <v>124</v>
       </c>
       <c r="N2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O2">
         <v>60267</v>
@@ -6590,7 +6624,7 @@
         <v>65536</v>
       </c>
       <c r="R2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S2">
         <v>2.1063333333299998</v>
@@ -6611,7 +6645,7 @@
         <v>126</v>
       </c>
       <c r="Y2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z2">
         <v>17027</v>
@@ -6623,7 +6657,7 @@
         <v>65536</v>
       </c>
       <c r="AC2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AD2">
         <v>7.4829999999999997</v>
@@ -6646,13 +6680,13 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
         <v>113</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>114</v>
-      </c>
-      <c r="C3" t="s">
-        <v>115</v>
       </c>
       <c r="D3">
         <v>8997</v>
@@ -6685,7 +6719,7 @@
         <v>125</v>
       </c>
       <c r="N3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O3">
         <v>57317</v>
@@ -6697,7 +6731,7 @@
         <v>65536</v>
       </c>
       <c r="R3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S3">
         <v>2.2126666666700001</v>
@@ -6718,7 +6752,7 @@
         <v>126</v>
       </c>
       <c r="Y3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z3">
         <v>18481</v>
@@ -6730,7 +6764,7 @@
         <v>65536</v>
       </c>
       <c r="AC3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AD3">
         <v>6.8860000000000001</v>
@@ -6753,13 +6787,13 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
         <v>113</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>115</v>
       </c>
       <c r="D4">
         <v>8570</v>
@@ -6792,7 +6826,7 @@
         <v>125</v>
       </c>
       <c r="N4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O4">
         <v>52732</v>
@@ -6804,7 +6838,7 @@
         <v>65536</v>
       </c>
       <c r="R4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S4">
         <v>2.4056666666700002</v>
@@ -6825,7 +6859,7 @@
         <v>126</v>
       </c>
       <c r="Y4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z4">
         <v>19153</v>
@@ -6837,7 +6871,7 @@
         <v>65536</v>
       </c>
       <c r="AC4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AD4">
         <v>6.6449999999999996</v>
@@ -6860,13 +6894,13 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
         <v>113</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>114</v>
-      </c>
-      <c r="C5" t="s">
-        <v>115</v>
       </c>
       <c r="D5">
         <v>7871</v>
@@ -6899,7 +6933,7 @@
         <v>125</v>
       </c>
       <c r="N5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O5">
         <v>51478</v>
@@ -6911,7 +6945,7 @@
         <v>65536</v>
       </c>
       <c r="R5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="S5">
         <v>2.4623333333300002</v>
@@ -6932,7 +6966,7 @@
         <v>126</v>
       </c>
       <c r="Y5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z5">
         <v>19764</v>
@@ -6944,7 +6978,7 @@
         <v>65536</v>
       </c>
       <c r="AC5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD5">
         <v>6.4393333333299996</v>
@@ -6967,13 +7001,13 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
         <v>113</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>114</v>
-      </c>
-      <c r="C6" t="s">
-        <v>115</v>
       </c>
       <c r="D6">
         <v>6853</v>
@@ -7006,7 +7040,7 @@
         <v>124</v>
       </c>
       <c r="N6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O6">
         <v>48993</v>
@@ -7018,7 +7052,7 @@
         <v>65536</v>
       </c>
       <c r="R6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S6">
         <v>2.5903333333299998</v>
@@ -7039,7 +7073,7 @@
         <v>126</v>
       </c>
       <c r="Y6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z6">
         <v>19712</v>
@@ -7051,7 +7085,7 @@
         <v>65536</v>
       </c>
       <c r="AC6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AD6">
         <v>6.4546666666699997</v>
@@ -7074,13 +7108,13 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
         <v>113</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>114</v>
-      </c>
-      <c r="C7" t="s">
-        <v>115</v>
       </c>
       <c r="D7">
         <v>9303</v>
@@ -7113,7 +7147,7 @@
         <v>123</v>
       </c>
       <c r="N7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O7">
         <v>47054</v>
@@ -7125,7 +7159,7 @@
         <v>65536</v>
       </c>
       <c r="R7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="S7">
         <v>2.6956666666700002</v>
@@ -7146,7 +7180,7 @@
         <v>126</v>
       </c>
       <c r="Y7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z7">
         <v>19788</v>
@@ -7158,7 +7192,7 @@
         <v>65536</v>
       </c>
       <c r="AC7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AD7">
         <v>6.4283333333300003</v>
@@ -7181,13 +7215,13 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
         <v>113</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>114</v>
-      </c>
-      <c r="C8" t="s">
-        <v>115</v>
       </c>
       <c r="D8">
         <v>7216</v>
@@ -7220,7 +7254,7 @@
         <v>125</v>
       </c>
       <c r="N8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O8">
         <v>42934</v>
@@ -7232,7 +7266,7 @@
         <v>65536</v>
       </c>
       <c r="R8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S8">
         <v>2.9540000000000002</v>
@@ -7253,7 +7287,7 @@
         <v>126</v>
       </c>
       <c r="Y8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z8">
         <v>18790</v>
@@ -7265,7 +7299,7 @@
         <v>65536</v>
       </c>
       <c r="AC8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AD8">
         <v>6.7686666666699997</v>
@@ -7288,13 +7322,13 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
         <v>113</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>114</v>
-      </c>
-      <c r="C9" t="s">
-        <v>115</v>
       </c>
       <c r="D9">
         <v>8643</v>
@@ -7327,7 +7361,7 @@
         <v>125</v>
       </c>
       <c r="N9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O9">
         <v>38865</v>
@@ -7339,7 +7373,7 @@
         <v>65536</v>
       </c>
       <c r="R9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S9">
         <v>3.26633333333</v>
@@ -7360,7 +7394,7 @@
         <v>126</v>
       </c>
       <c r="Y9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z9">
         <v>17559</v>
@@ -7372,7 +7406,7 @@
         <v>65536</v>
       </c>
       <c r="AC9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AD9">
         <v>7.2423333333300004</v>
@@ -7395,13 +7429,13 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
         <v>113</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>114</v>
-      </c>
-      <c r="C10" t="s">
-        <v>115</v>
       </c>
       <c r="D10">
         <v>8431</v>
@@ -7434,7 +7468,7 @@
         <v>126</v>
       </c>
       <c r="N10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O10">
         <v>35170</v>
@@ -7446,7 +7480,7 @@
         <v>65536</v>
       </c>
       <c r="R10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S10">
         <v>3.6153333333300002</v>
@@ -7467,7 +7501,7 @@
         <v>126</v>
       </c>
       <c r="Y10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z10">
         <v>16162</v>
@@ -7479,7 +7513,7 @@
         <v>65536</v>
       </c>
       <c r="AC10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AD10">
         <v>7.8673333333300004</v>
@@ -7502,13 +7536,13 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
         <v>113</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>114</v>
-      </c>
-      <c r="C11" t="s">
-        <v>115</v>
       </c>
       <c r="D11">
         <v>10134</v>
@@ -7541,7 +7575,7 @@
         <v>125</v>
       </c>
       <c r="N11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O11">
         <v>31849</v>
@@ -7553,7 +7587,7 @@
         <v>65536</v>
       </c>
       <c r="R11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S11">
         <v>3.99633333333</v>
@@ -7574,7 +7608,7 @@
         <v>126</v>
       </c>
       <c r="Y11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z11">
         <v>15215</v>
@@ -7586,7 +7620,7 @@
         <v>65536</v>
       </c>
       <c r="AC11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AD11">
         <v>8.3573333333300006</v>
@@ -7609,13 +7643,13 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
         <v>113</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>114</v>
-      </c>
-      <c r="C12" t="s">
-        <v>115</v>
       </c>
       <c r="D12">
         <v>9700</v>
@@ -7648,7 +7682,7 @@
         <v>127</v>
       </c>
       <c r="N12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O12">
         <v>29482</v>
@@ -7660,7 +7694,7 @@
         <v>65536</v>
       </c>
       <c r="R12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S12">
         <v>4.3016666666700001</v>
@@ -7681,7 +7715,7 @@
         <v>126</v>
       </c>
       <c r="Y12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Z12">
         <v>14265</v>
@@ -7693,7 +7727,7 @@
         <v>65536</v>
       </c>
       <c r="AC12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AD12">
         <v>8.9133333333299998</v>
@@ -7721,21 +7755,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100050FBA8A9F0AFB4BB2D0148D6A234C38" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74183e733b66e5e9a3cd5553bd4bd9ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4a052287-e6d5-446a-afc6-58987b850d5f" xmlns:ns4="943a090e-7b96-4eb7-abc0-264fa36c6c5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6b903754823e47922d1d3c75b6236d24" ns3:_="" ns4:_="">
     <xsd:import namespace="4a052287-e6d5-446a-afc6-58987b850d5f"/>
@@ -7958,32 +7977,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7769B51B-49EA-4054-A0C2-A13FF67FB754}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="4a052287-e6d5-446a-afc6-58987b850d5f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="943a090e-7b96-4eb7-abc0-264fa36c6c5d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEC18BF-42E1-4B07-B0F9-328B1505E1A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{097D0541-97F4-46BE-8711-51CFA8DE5931}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8000,4 +8009,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEEC18BF-42E1-4B07-B0F9-328B1505E1A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7769B51B-49EA-4054-A0C2-A13FF67FB754}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="4a052287-e6d5-446a-afc6-58987b850d5f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="943a090e-7b96-4eb7-abc0-264fa36c6c5d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>